<commit_message>
iiii i iii i
</commit_message>
<xml_diff>
--- a/SAE_3_01/fichiers genere/S1.xlsx
+++ b/SAE_3_01/fichiers genere/S1.xlsx
@@ -4361,7 +4361,7 @@
       </c>
       <c r="G2" s="28" t="inlineStr">
         <is>
-          <t>Josée VAQUIERI PORTOLANO</t>
+          <t>JosÃ©e VAQUIERI PORTOLANO</t>
         </is>
       </c>
       <c r="H2" s="28" t="n"/>
@@ -13316,7 +13316,7 @@
       </c>
       <c r="G2" s="28" t="inlineStr">
         <is>
-          <t>Mickaël MARTIN NEVOT</t>
+          <t>MickaÃ«l MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="28" t="n"/>
@@ -15107,7 +15107,7 @@
       </c>
       <c r="G2" s="28" t="inlineStr">
         <is>
-          <t>Mickaël MARTIN NEVOT</t>
+          <t>MickaÃ«l MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="28" t="n"/>
@@ -16898,7 +16898,7 @@
       </c>
       <c r="G2" s="28" t="inlineStr">
         <is>
-          <t>Mickaël MARTIN NEVOT</t>
+          <t>MickaÃ«l MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="28" t="n"/>
@@ -18689,7 +18689,7 @@
       </c>
       <c r="G2" s="28" t="inlineStr">
         <is>
-          <t>Mickaël MARTIN NEVOT</t>
+          <t>MickaÃ«l MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="28" t="n"/>

</xml_diff>

<commit_message>
écriture de chaque cours avec la date etc le nombre d'heure
</commit_message>
<xml_diff>
--- a/SAE_3_01/fichiers genere/S1.xlsx
+++ b/SAE_3_01/fichiers genere/S1.xlsx
@@ -3307,9 +3307,21 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="n"/>
-      <c r="B35" s="29" t="n"/>
-      <c r="C35" s="28" t="n"/>
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="B35" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C35" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
@@ -3327,9 +3339,17 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="n"/>
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-20</t>
+        </is>
+      </c>
       <c r="B36" s="29" t="n"/>
-      <c r="C36" s="28" t="n"/>
+      <c r="C36" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
@@ -3347,9 +3367,17 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="n"/>
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
       <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="n"/>
+      <c r="C37" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
@@ -3367,9 +3395,17 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="n"/>
+      <c r="A38" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-04</t>
+        </is>
+      </c>
       <c r="B38" s="28" t="n"/>
-      <c r="C38" s="28" t="n"/>
+      <c r="C38" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
@@ -3387,9 +3423,17 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="n"/>
+      <c r="A39" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-11</t>
+        </is>
+      </c>
       <c r="B39" s="28" t="n"/>
-      <c r="C39" s="28" t="n"/>
+      <c r="C39" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
@@ -3407,9 +3451,17 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="n"/>
+      <c r="A40" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B40" s="28" t="n"/>
-      <c r="C40" s="28" t="n"/>
+      <c r="C40" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D40" s="28" t="n"/>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
@@ -3427,10 +3479,22 @@
       <c r="R40" s="28" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="n"/>
+      <c r="A41" s="28" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
       <c r="B41" s="28" t="n"/>
-      <c r="C41" s="28" t="n"/>
-      <c r="D41" s="28" t="n"/>
+      <c r="C41" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
+      <c r="D41" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
       <c r="G41" s="28" t="n"/>
@@ -5098,10 +5162,18 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="n"/>
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-04</t>
+        </is>
+      </c>
       <c r="B35" s="29" t="n"/>
       <c r="C35" s="28" t="n"/>
-      <c r="D35" s="28" t="n"/>
+      <c r="D35" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
       <c r="G35" s="28" t="n"/>
@@ -5118,10 +5190,18 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="n"/>
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-11</t>
+        </is>
+      </c>
       <c r="B36" s="29" t="n"/>
       <c r="C36" s="28" t="n"/>
-      <c r="D36" s="28" t="n"/>
+      <c r="D36" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
       <c r="G36" s="28" t="n"/>
@@ -5138,10 +5218,18 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="n"/>
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-18</t>
+        </is>
+      </c>
       <c r="B37" s="29" t="n"/>
       <c r="C37" s="28" t="n"/>
-      <c r="D37" s="28" t="n"/>
+      <c r="D37" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
       <c r="G37" s="28" t="n"/>
@@ -5158,10 +5246,18 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="n"/>
+      <c r="A38" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-25</t>
+        </is>
+      </c>
       <c r="B38" s="28" t="n"/>
       <c r="C38" s="28" t="n"/>
-      <c r="D38" s="28" t="n"/>
+      <c r="D38" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
       <c r="G38" s="28" t="n"/>
@@ -5178,10 +5274,18 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="n"/>
+      <c r="A39" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-09</t>
+        </is>
+      </c>
       <c r="B39" s="28" t="n"/>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="n"/>
+      <c r="D39" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -5198,10 +5302,18 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="n"/>
+      <c r="A40" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-16</t>
+        </is>
+      </c>
       <c r="B40" s="28" t="n"/>
       <c r="C40" s="28" t="n"/>
-      <c r="D40" s="28" t="n"/>
+      <c r="D40" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
       <c r="G40" s="28" t="n"/>
@@ -5218,10 +5330,18 @@
       <c r="R40" s="28" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="n"/>
+      <c r="A41" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-23</t>
+        </is>
+      </c>
       <c r="B41" s="28" t="n"/>
       <c r="C41" s="28" t="n"/>
-      <c r="D41" s="28" t="n"/>
+      <c r="D41" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
       <c r="G41" s="28" t="n"/>
@@ -5238,10 +5358,18 @@
       <c r="R41" s="28" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="28" t="n"/>
+      <c r="A42" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
       <c r="B42" s="28" t="n"/>
       <c r="C42" s="28" t="n"/>
-      <c r="D42" s="28" t="n"/>
+      <c r="D42" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E42" s="28" t="n"/>
       <c r="F42" s="28" t="n"/>
       <c r="G42" s="28" t="n"/>
@@ -5258,10 +5386,18 @@
       <c r="R42" s="28" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="28" t="n"/>
+      <c r="A43" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
       <c r="B43" s="28" t="n"/>
       <c r="C43" s="28" t="n"/>
-      <c r="D43" s="28" t="n"/>
+      <c r="D43" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E43" s="28" t="n"/>
       <c r="F43" s="28" t="n"/>
       <c r="G43" s="28" t="n"/>
@@ -5278,10 +5414,18 @@
       <c r="R43" s="28" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="28" t="n"/>
+      <c r="A44" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-20</t>
+        </is>
+      </c>
       <c r="B44" s="28" t="n"/>
       <c r="C44" s="28" t="n"/>
-      <c r="D44" s="28" t="n"/>
+      <c r="D44" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E44" s="28" t="n"/>
       <c r="F44" s="28" t="n"/>
       <c r="G44" s="28" t="n"/>
@@ -5298,10 +5442,18 @@
       <c r="R44" s="28" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="28" t="n"/>
+      <c r="A45" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
       <c r="B45" s="28" t="n"/>
       <c r="C45" s="28" t="n"/>
-      <c r="D45" s="28" t="n"/>
+      <c r="D45" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E45" s="28" t="n"/>
       <c r="F45" s="28" t="n"/>
       <c r="G45" s="28" t="n"/>
@@ -5318,10 +5470,18 @@
       <c r="R45" s="28" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="28" t="n"/>
+      <c r="A46" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-04</t>
+        </is>
+      </c>
       <c r="B46" s="28" t="n"/>
       <c r="C46" s="28" t="n"/>
-      <c r="D46" s="28" t="n"/>
+      <c r="D46" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E46" s="28" t="n"/>
       <c r="F46" s="28" t="n"/>
       <c r="G46" s="28" t="n"/>
@@ -5338,10 +5498,18 @@
       <c r="R46" s="28" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="28" t="n"/>
+      <c r="A47" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-11</t>
+        </is>
+      </c>
       <c r="B47" s="28" t="n"/>
       <c r="C47" s="28" t="n"/>
-      <c r="D47" s="28" t="n"/>
+      <c r="D47" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E47" s="28" t="n"/>
       <c r="F47" s="28" t="n"/>
       <c r="G47" s="28" t="n"/>
@@ -6889,9 +7057,17 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="n"/>
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-11</t>
+        </is>
+      </c>
       <c r="B35" s="29" t="n"/>
-      <c r="C35" s="28" t="n"/>
+      <c r="C35" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
@@ -6909,9 +7085,17 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="n"/>
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-18</t>
+        </is>
+      </c>
       <c r="B36" s="29" t="n"/>
-      <c r="C36" s="28" t="n"/>
+      <c r="C36" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
@@ -6929,9 +7113,17 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="n"/>
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-25</t>
+        </is>
+      </c>
       <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="n"/>
+      <c r="C37" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
@@ -6949,9 +7141,17 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="n"/>
+      <c r="A38" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-09</t>
+        </is>
+      </c>
       <c r="B38" s="28" t="n"/>
-      <c r="C38" s="28" t="n"/>
+      <c r="C38" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
@@ -6969,9 +7169,17 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="n"/>
+      <c r="A39" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-16</t>
+        </is>
+      </c>
       <c r="B39" s="28" t="n"/>
-      <c r="C39" s="28" t="n"/>
+      <c r="C39" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
@@ -6989,9 +7197,17 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="n"/>
+      <c r="A40" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-23</t>
+        </is>
+      </c>
       <c r="B40" s="28" t="n"/>
-      <c r="C40" s="28" t="n"/>
+      <c r="C40" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D40" s="28" t="n"/>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
@@ -7009,9 +7225,17 @@
       <c r="R40" s="28" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="n"/>
+      <c r="A41" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
       <c r="B41" s="28" t="n"/>
-      <c r="C41" s="28" t="n"/>
+      <c r="C41" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D41" s="28" t="n"/>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
@@ -7029,9 +7253,17 @@
       <c r="R41" s="28" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="28" t="n"/>
+      <c r="A42" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
       <c r="B42" s="28" t="n"/>
-      <c r="C42" s="28" t="n"/>
+      <c r="C42" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D42" s="28" t="n"/>
       <c r="E42" s="28" t="n"/>
       <c r="F42" s="28" t="n"/>
@@ -7049,9 +7281,17 @@
       <c r="R42" s="28" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="28" t="n"/>
+      <c r="A43" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-20</t>
+        </is>
+      </c>
       <c r="B43" s="28" t="n"/>
-      <c r="C43" s="28" t="n"/>
+      <c r="C43" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D43" s="28" t="n"/>
       <c r="E43" s="28" t="n"/>
       <c r="F43" s="28" t="n"/>
@@ -7069,9 +7309,17 @@
       <c r="R43" s="28" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="28" t="n"/>
+      <c r="A44" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
       <c r="B44" s="28" t="n"/>
-      <c r="C44" s="28" t="n"/>
+      <c r="C44" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D44" s="28" t="n"/>
       <c r="E44" s="28" t="n"/>
       <c r="F44" s="28" t="n"/>
@@ -8680,9 +8928,17 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="n"/>
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
       <c r="B35" s="29" t="n"/>
-      <c r="C35" s="28" t="n"/>
+      <c r="C35" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
@@ -8700,9 +8956,17 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="n"/>
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-04</t>
+        </is>
+      </c>
       <c r="B36" s="29" t="n"/>
-      <c r="C36" s="28" t="n"/>
+      <c r="C36" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
@@ -8720,9 +8984,17 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="n"/>
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-11</t>
+        </is>
+      </c>
       <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="n"/>
+      <c r="C37" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
@@ -8740,9 +9012,17 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="n"/>
+      <c r="A38" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B38" s="28" t="n"/>
-      <c r="C38" s="28" t="n"/>
+      <c r="C38" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
@@ -8760,10 +9040,18 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="n"/>
+      <c r="A39" s="28" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
       <c r="B39" s="28" t="n"/>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="n"/>
+      <c r="D39" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -11661,7 +11949,11 @@
       <c r="R7" s="28" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="29" t="n"/>
+      <c r="A8" s="29" t="inlineStr">
+        <is>
+          <t>Alain Casali</t>
+        </is>
+      </c>
       <c r="C8" s="28" t="n"/>
       <c r="D8" s="28" t="n"/>
       <c r="E8" s="28" t="n"/>
@@ -11680,7 +11972,11 @@
       <c r="R8" s="28" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="29" t="n"/>
+      <c r="A9" s="29" t="inlineStr">
+        <is>
+          <t>Christian Ernst</t>
+        </is>
+      </c>
       <c r="C9" s="28" t="n"/>
       <c r="D9" s="28" t="n"/>
       <c r="E9" s="28" t="n"/>
@@ -11699,7 +11995,11 @@
       <c r="R9" s="28" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="29" t="n"/>
+      <c r="A10" s="29" t="inlineStr">
+        <is>
+          <t>Basma Boukenze</t>
+        </is>
+      </c>
       <c r="C10" s="28" t="n"/>
       <c r="D10" s="28" t="n"/>
       <c r="E10" s="28" t="n"/>
@@ -11819,7 +12119,11 @@
       <c r="R14" s="28" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="n"/>
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>Alain Casali</t>
+        </is>
+      </c>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="28" t="n"/>
       <c r="D15" s="33" t="inlineStr">
@@ -11847,7 +12151,11 @@
       <c r="R15" s="28" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="10" t="n"/>
+      <c r="A16" s="10" t="inlineStr">
+        <is>
+          <t>Christian Ernst</t>
+        </is>
+      </c>
       <c r="B16" s="11" t="n"/>
       <c r="C16" s="28" t="n"/>
       <c r="D16" s="28" t="n"/>
@@ -11891,8 +12199,14 @@
       <c r="R17" s="28" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="8" t="n"/>
-      <c r="B18" s="13" t="n"/>
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>Alain Casali</t>
+        </is>
+      </c>
+      <c r="B18" s="13" t="n">
+        <v>2</v>
+      </c>
       <c r="C18" s="28" t="n"/>
       <c r="D18" s="28" t="n"/>
       <c r="E18" s="28" t="n"/>
@@ -11911,8 +12225,14 @@
       <c r="R18" s="28" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="n"/>
-      <c r="B19" s="13" t="n"/>
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>Christian Ernst</t>
+        </is>
+      </c>
+      <c r="B19" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="C19" s="28" t="n"/>
       <c r="D19" s="39" t="inlineStr">
         <is>
@@ -11935,8 +12255,14 @@
       <c r="R19" s="28" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="8" t="n"/>
-      <c r="B20" s="13" t="n"/>
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>Basma Boukenze</t>
+        </is>
+      </c>
+      <c r="B20" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="C20" s="28" t="n"/>
       <c r="D20" s="41" t="inlineStr">
         <is>
@@ -12011,8 +12337,14 @@
       <c r="R22" s="28" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="8" t="n"/>
-      <c r="B23" s="8" t="n"/>
+      <c r="A23" s="8" t="inlineStr">
+        <is>
+          <t>Alain Casali</t>
+        </is>
+      </c>
+      <c r="B23" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="C23" s="28" t="n"/>
       <c r="D23" s="28" t="n"/>
       <c r="E23" s="28" t="n"/>
@@ -12031,8 +12363,14 @@
       <c r="R23" s="28" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="8" t="n"/>
-      <c r="B24" s="8" t="n"/>
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>Christian Ernst</t>
+        </is>
+      </c>
+      <c r="B24" s="8" t="n">
+        <v>2</v>
+      </c>
       <c r="C24" s="28" t="n"/>
       <c r="D24" s="28" t="n"/>
       <c r="E24" s="28" t="n"/>
@@ -12051,8 +12389,14 @@
       <c r="R24" s="28" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="8" t="n"/>
-      <c r="B25" s="8" t="n"/>
+      <c r="A25" s="8" t="inlineStr">
+        <is>
+          <t>Basma Boukenze</t>
+        </is>
+      </c>
+      <c r="B25" s="8" t="n">
+        <v>2</v>
+      </c>
       <c r="C25" s="28" t="n"/>
       <c r="D25" s="28" t="n"/>
       <c r="G25" s="28" t="n"/>
@@ -12117,8 +12461,14 @@
       <c r="R27" s="28" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="8" t="n"/>
-      <c r="B28" s="13" t="n"/>
+      <c r="A28" s="8" t="inlineStr">
+        <is>
+          <t>Alain Casali</t>
+        </is>
+      </c>
+      <c r="B28" s="13" t="n">
+        <v>2</v>
+      </c>
       <c r="C28" s="28" t="n"/>
       <c r="D28" s="62" t="inlineStr">
         <is>
@@ -12140,8 +12490,14 @@
       <c r="R28" s="28" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="8" t="n"/>
-      <c r="B29" s="13" t="n"/>
+      <c r="A29" s="8" t="inlineStr">
+        <is>
+          <t>Christian Ernst</t>
+        </is>
+      </c>
+      <c r="B29" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="C29" s="28" t="n"/>
       <c r="D29" s="63" t="n"/>
       <c r="H29" s="61" t="n"/>
@@ -12157,8 +12513,14 @@
       <c r="R29" s="28" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="8" t="n"/>
-      <c r="B30" s="13" t="n"/>
+      <c r="A30" s="8" t="inlineStr">
+        <is>
+          <t>Basma Boukenze</t>
+        </is>
+      </c>
+      <c r="B30" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="C30" s="28" t="n"/>
       <c r="D30" s="63" t="n"/>
       <c r="H30" s="61" t="n"/>
@@ -12262,8 +12624,16 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="n"/>
-      <c r="B35" s="29" t="n"/>
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-04</t>
+        </is>
+      </c>
+      <c r="B35" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 4H</t>
+        </is>
+      </c>
       <c r="C35" s="28" t="n"/>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
@@ -12282,9 +12652,21 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="n"/>
-      <c r="B36" s="29" t="n"/>
-      <c r="C36" s="28" t="n"/>
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-11</t>
+        </is>
+      </c>
+      <c r="B36" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 4H</t>
+        </is>
+      </c>
+      <c r="C36" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
@@ -12302,9 +12684,21 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="n"/>
-      <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="n"/>
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-18</t>
+        </is>
+      </c>
+      <c r="B37" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 4H</t>
+        </is>
+      </c>
+      <c r="C37" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
@@ -12322,10 +12716,26 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="n"/>
-      <c r="B38" s="28" t="n"/>
-      <c r="C38" s="28" t="n"/>
-      <c r="D38" s="28" t="n"/>
+      <c r="A38" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-25</t>
+        </is>
+      </c>
+      <c r="B38" s="28" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C38" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
+      <c r="D38" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
       <c r="G38" s="28" t="n"/>
@@ -12342,10 +12752,26 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="n"/>
-      <c r="B39" s="28" t="n"/>
-      <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="n"/>
+      <c r="A39" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-02</t>
+        </is>
+      </c>
+      <c r="B39" s="28" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C39" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
+      <c r="D39" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -12362,10 +12788,26 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="n"/>
-      <c r="B40" s="28" t="n"/>
-      <c r="C40" s="28" t="n"/>
-      <c r="D40" s="28" t="n"/>
+      <c r="A40" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-09</t>
+        </is>
+      </c>
+      <c r="B40" s="28" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C40" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
+      <c r="D40" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
       <c r="G40" s="28" t="n"/>
@@ -12382,10 +12824,22 @@
       <c r="R40" s="28" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="n"/>
+      <c r="A41" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-16</t>
+        </is>
+      </c>
       <c r="B41" s="28" t="n"/>
-      <c r="C41" s="28" t="n"/>
-      <c r="D41" s="28" t="n"/>
+      <c r="C41" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
+      <c r="D41" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
       <c r="G41" s="28" t="n"/>
@@ -12402,10 +12856,26 @@
       <c r="R41" s="28" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="28" t="n"/>
-      <c r="B42" s="28" t="n"/>
-      <c r="C42" s="28" t="n"/>
-      <c r="D42" s="28" t="n"/>
+      <c r="A42" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-23</t>
+        </is>
+      </c>
+      <c r="B42" s="28" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C42" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
+      <c r="D42" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E42" s="28" t="n"/>
       <c r="F42" s="28" t="n"/>
       <c r="G42" s="28" t="n"/>
@@ -12422,10 +12892,22 @@
       <c r="R42" s="28" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="28" t="n"/>
+      <c r="A43" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
       <c r="B43" s="28" t="n"/>
-      <c r="C43" s="28" t="n"/>
-      <c r="D43" s="28" t="n"/>
+      <c r="C43" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
+      <c r="D43" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E43" s="28" t="n"/>
       <c r="F43" s="28" t="n"/>
       <c r="G43" s="28" t="n"/>
@@ -12442,10 +12924,26 @@
       <c r="R43" s="28" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="28" t="n"/>
-      <c r="B44" s="28" t="n"/>
-      <c r="C44" s="28" t="n"/>
-      <c r="D44" s="28" t="n"/>
+      <c r="A44" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="B44" s="28" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C44" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
+      <c r="D44" s="28" t="inlineStr">
+        <is>
+          <t>TP 6H</t>
+        </is>
+      </c>
       <c r="E44" s="28" t="n"/>
       <c r="F44" s="28" t="n"/>
       <c r="G44" s="28" t="n"/>
@@ -12462,10 +12960,22 @@
       <c r="R44" s="28" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="28" t="n"/>
+      <c r="A45" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-20</t>
+        </is>
+      </c>
       <c r="B45" s="28" t="n"/>
-      <c r="C45" s="28" t="n"/>
-      <c r="D45" s="28" t="n"/>
+      <c r="C45" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
+      <c r="D45" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E45" s="28" t="n"/>
       <c r="F45" s="28" t="n"/>
       <c r="G45" s="28" t="n"/>
@@ -12482,10 +12992,26 @@
       <c r="R45" s="28" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="28" t="n"/>
-      <c r="B46" s="28" t="n"/>
-      <c r="C46" s="28" t="n"/>
-      <c r="D46" s="28" t="n"/>
+      <c r="A46" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
+      <c r="B46" s="28" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C46" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
+      <c r="D46" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E46" s="28" t="n"/>
       <c r="F46" s="28" t="n"/>
       <c r="G46" s="28" t="n"/>
@@ -12502,10 +13028,18 @@
       <c r="R46" s="28" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="28" t="n"/>
+      <c r="A47" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-04</t>
+        </is>
+      </c>
       <c r="B47" s="28" t="n"/>
       <c r="C47" s="28" t="n"/>
-      <c r="D47" s="28" t="n"/>
+      <c r="D47" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E47" s="28" t="n"/>
       <c r="F47" s="28" t="n"/>
       <c r="G47" s="28" t="n"/>
@@ -12522,10 +13056,18 @@
       <c r="R47" s="28" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="28" t="n"/>
+      <c r="A48" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-11</t>
+        </is>
+      </c>
       <c r="B48" s="28" t="n"/>
       <c r="C48" s="28" t="n"/>
-      <c r="D48" s="28" t="n"/>
+      <c r="D48" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E48" s="28" t="n"/>
       <c r="F48" s="28" t="n"/>
       <c r="G48" s="28" t="n"/>
@@ -12542,10 +13084,18 @@
       <c r="R48" s="28" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="28" t="n"/>
+      <c r="A49" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B49" s="28" t="n"/>
       <c r="C49" s="28" t="n"/>
-      <c r="D49" s="28" t="n"/>
+      <c r="D49" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E49" s="28" t="n"/>
       <c r="F49" s="28" t="n"/>
       <c r="G49" s="28" t="n"/>
@@ -12562,7 +13112,11 @@
       <c r="R49" s="28" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="28" t="n"/>
+      <c r="A50" s="28" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
       <c r="B50" s="28" t="n"/>
       <c r="C50" s="28" t="n"/>
       <c r="D50" s="28" t="n"/>
@@ -13452,7 +14006,11 @@
       <c r="R7" s="28" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="29" t="n"/>
+      <c r="A8" s="29" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
       <c r="C8" s="28" t="n"/>
       <c r="D8" s="28" t="n"/>
       <c r="E8" s="28" t="n"/>
@@ -13471,7 +14029,11 @@
       <c r="R8" s="28" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="29" t="n"/>
+      <c r="A9" s="29" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
       <c r="C9" s="28" t="n"/>
       <c r="D9" s="28" t="n"/>
       <c r="E9" s="28" t="n"/>
@@ -13610,7 +14172,11 @@
       <c r="R14" s="28" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="n"/>
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="28" t="n"/>
       <c r="D15" s="33" t="inlineStr">
@@ -13682,8 +14248,14 @@
       <c r="R17" s="28" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="8" t="n"/>
-      <c r="B18" s="13" t="n"/>
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
+      <c r="B18" s="13" t="n">
+        <v>2</v>
+      </c>
       <c r="C18" s="28" t="n"/>
       <c r="D18" s="28" t="n"/>
       <c r="E18" s="28" t="n"/>
@@ -13702,8 +14274,14 @@
       <c r="R18" s="28" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="n"/>
-      <c r="B19" s="13" t="n"/>
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="B19" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="C19" s="28" t="n"/>
       <c r="D19" s="39" t="inlineStr">
         <is>
@@ -13802,8 +14380,14 @@
       <c r="R22" s="28" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="8" t="n"/>
-      <c r="B23" s="8" t="n"/>
+      <c r="A23" s="8" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
+      <c r="B23" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="C23" s="28" t="n"/>
       <c r="D23" s="28" t="n"/>
       <c r="E23" s="28" t="n"/>
@@ -13822,8 +14406,14 @@
       <c r="R23" s="28" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="8" t="n"/>
-      <c r="B24" s="8" t="n"/>
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="B24" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="C24" s="28" t="n"/>
       <c r="D24" s="28" t="n"/>
       <c r="E24" s="28" t="n"/>
@@ -13908,8 +14498,14 @@
       <c r="R27" s="28" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="8" t="n"/>
-      <c r="B28" s="13" t="n"/>
+      <c r="A28" s="8" t="inlineStr">
+        <is>
+          <t>Test2</t>
+        </is>
+      </c>
+      <c r="B28" s="13" t="n">
+        <v>3</v>
+      </c>
       <c r="C28" s="28" t="n"/>
       <c r="D28" s="62" t="inlineStr">
         <is>
@@ -13931,8 +14527,14 @@
       <c r="R28" s="28" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="8" t="n"/>
-      <c r="B29" s="13" t="n"/>
+      <c r="A29" s="8" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="B29" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="C29" s="28" t="n"/>
       <c r="D29" s="63" t="n"/>
       <c r="H29" s="61" t="n"/>
@@ -14053,8 +14655,16 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="n"/>
-      <c r="B35" s="29" t="n"/>
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
+      <c r="B35" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 4H</t>
+        </is>
+      </c>
       <c r="C35" s="28" t="n"/>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
@@ -14073,10 +14683,22 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="n"/>
-      <c r="B36" s="29" t="n"/>
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-04</t>
+        </is>
+      </c>
+      <c r="B36" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
       <c r="C36" s="28" t="n"/>
-      <c r="D36" s="28" t="n"/>
+      <c r="D36" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
       <c r="G36" s="28" t="n"/>
@@ -14093,10 +14715,18 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="n"/>
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-11</t>
+        </is>
+      </c>
       <c r="B37" s="29" t="n"/>
       <c r="C37" s="28" t="n"/>
-      <c r="D37" s="28" t="n"/>
+      <c r="D37" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
       <c r="G37" s="28" t="n"/>
@@ -14113,10 +14743,18 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="n"/>
+      <c r="A38" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B38" s="28" t="n"/>
       <c r="C38" s="28" t="n"/>
-      <c r="D38" s="28" t="n"/>
+      <c r="D38" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
       <c r="G38" s="28" t="n"/>
@@ -14133,10 +14771,18 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="n"/>
+      <c r="A39" s="28" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
       <c r="B39" s="28" t="n"/>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="n"/>
+      <c r="D39" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -15844,8 +16490,16 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="n"/>
-      <c r="B35" s="29" t="n"/>
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-18</t>
+        </is>
+      </c>
+      <c r="B35" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
       <c r="C35" s="28" t="n"/>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
@@ -15864,8 +16518,16 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="n"/>
-      <c r="B36" s="29" t="n"/>
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-25</t>
+        </is>
+      </c>
+      <c r="B36" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
       <c r="C36" s="28" t="n"/>
       <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
@@ -15884,9 +16546,17 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="n"/>
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-02</t>
+        </is>
+      </c>
       <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="n"/>
+      <c r="C37" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
@@ -15904,10 +16574,18 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="n"/>
+      <c r="A38" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-09</t>
+        </is>
+      </c>
       <c r="B38" s="28" t="n"/>
       <c r="C38" s="28" t="n"/>
-      <c r="D38" s="28" t="n"/>
+      <c r="D38" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
       <c r="G38" s="28" t="n"/>
@@ -15924,10 +16602,18 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="n"/>
+      <c r="A39" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-16</t>
+        </is>
+      </c>
       <c r="B39" s="28" t="n"/>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="n"/>
+      <c r="D39" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -15944,7 +16630,11 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="n"/>
+      <c r="A40" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-23</t>
+        </is>
+      </c>
       <c r="B40" s="28" t="n"/>
       <c r="C40" s="28" t="n"/>
       <c r="D40" s="28" t="n"/>
@@ -17635,10 +18325,22 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="n"/>
-      <c r="B35" s="29" t="n"/>
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-04</t>
+        </is>
+      </c>
+      <c r="B35" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 4H</t>
+        </is>
+      </c>
       <c r="C35" s="28" t="n"/>
-      <c r="D35" s="28" t="n"/>
+      <c r="D35" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
       <c r="G35" s="28" t="n"/>
@@ -17655,10 +18357,22 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="n"/>
-      <c r="B36" s="29" t="n"/>
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-11</t>
+        </is>
+      </c>
+      <c r="B36" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
       <c r="C36" s="28" t="n"/>
-      <c r="D36" s="28" t="n"/>
+      <c r="D36" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
       <c r="G36" s="28" t="n"/>
@@ -17675,10 +18389,18 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="n"/>
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-18</t>
+        </is>
+      </c>
       <c r="B37" s="29" t="n"/>
       <c r="C37" s="28" t="n"/>
-      <c r="D37" s="28" t="n"/>
+      <c r="D37" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
       <c r="G37" s="28" t="n"/>
@@ -17695,10 +18417,18 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="n"/>
+      <c r="A38" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-25</t>
+        </is>
+      </c>
       <c r="B38" s="28" t="n"/>
       <c r="C38" s="28" t="n"/>
-      <c r="D38" s="28" t="n"/>
+      <c r="D38" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
       <c r="G38" s="28" t="n"/>
@@ -17715,9 +18445,17 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="n"/>
+      <c r="A39" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-02</t>
+        </is>
+      </c>
       <c r="B39" s="28" t="n"/>
-      <c r="C39" s="28" t="n"/>
+      <c r="C39" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
@@ -18825,7 +19563,11 @@
       <c r="R7" s="28" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="29" t="n"/>
+      <c r="A8" s="29" t="inlineStr">
+        <is>
+          <t>zzz</t>
+        </is>
+      </c>
       <c r="C8" s="28" t="n"/>
       <c r="D8" s="28" t="n"/>
       <c r="E8" s="28" t="n"/>
@@ -18983,7 +19725,11 @@
       <c r="R14" s="28" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="n"/>
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>zzz</t>
+        </is>
+      </c>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="28" t="n"/>
       <c r="D15" s="33" t="inlineStr">
@@ -19055,8 +19801,14 @@
       <c r="R17" s="28" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="8" t="n"/>
-      <c r="B18" s="13" t="n"/>
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>zzz</t>
+        </is>
+      </c>
+      <c r="B18" s="13" t="n">
+        <v>3</v>
+      </c>
       <c r="C18" s="28" t="n"/>
       <c r="D18" s="28" t="n"/>
       <c r="E18" s="28" t="n"/>
@@ -19175,8 +19927,14 @@
       <c r="R22" s="28" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="8" t="n"/>
-      <c r="B23" s="8" t="n"/>
+      <c r="A23" s="8" t="inlineStr">
+        <is>
+          <t>zzz</t>
+        </is>
+      </c>
+      <c r="B23" s="8" t="n">
+        <v>2</v>
+      </c>
       <c r="C23" s="28" t="n"/>
       <c r="D23" s="28" t="n"/>
       <c r="E23" s="28" t="n"/>
@@ -19281,8 +20039,14 @@
       <c r="R27" s="28" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="8" t="n"/>
-      <c r="B28" s="13" t="n"/>
+      <c r="A28" s="8" t="inlineStr">
+        <is>
+          <t>zzz</t>
+        </is>
+      </c>
+      <c r="B28" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="C28" s="28" t="n"/>
       <c r="D28" s="62" t="inlineStr">
         <is>
@@ -19426,8 +20190,16 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="n"/>
-      <c r="B35" s="29" t="n"/>
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-09</t>
+        </is>
+      </c>
+      <c r="B35" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
       <c r="C35" s="28" t="n"/>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
@@ -19446,8 +20218,16 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="n"/>
-      <c r="B36" s="29" t="n"/>
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-16</t>
+        </is>
+      </c>
+      <c r="B36" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
       <c r="C36" s="28" t="n"/>
       <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
@@ -19466,10 +20246,22 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="n"/>
-      <c r="B37" s="29" t="n"/>
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-23</t>
+        </is>
+      </c>
+      <c r="B37" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
       <c r="C37" s="28" t="n"/>
-      <c r="D37" s="28" t="n"/>
+      <c r="D37" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
       <c r="G37" s="28" t="n"/>
@@ -19486,10 +20278,22 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="n"/>
-      <c r="B38" s="28" t="n"/>
+      <c r="A38" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
+      <c r="B38" s="28" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
       <c r="C38" s="28" t="n"/>
-      <c r="D38" s="28" t="n"/>
+      <c r="D38" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
       <c r="G38" s="28" t="n"/>
@@ -19506,10 +20310,22 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="n"/>
-      <c r="B39" s="28" t="n"/>
+      <c r="A39" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="B39" s="28" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="n"/>
+      <c r="D39" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -19526,10 +20342,18 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="n"/>
+      <c r="A40" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
       <c r="B40" s="28" t="n"/>
       <c r="C40" s="28" t="n"/>
-      <c r="D40" s="28" t="n"/>
+      <c r="D40" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
       <c r="G40" s="28" t="n"/>
@@ -19546,9 +20370,17 @@
       <c r="R40" s="28" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="n"/>
+      <c r="A41" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-04</t>
+        </is>
+      </c>
       <c r="B41" s="28" t="n"/>
-      <c r="C41" s="28" t="n"/>
+      <c r="C41" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D41" s="28" t="n"/>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
@@ -19566,9 +20398,17 @@
       <c r="R41" s="28" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="28" t="n"/>
+      <c r="A42" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-11</t>
+        </is>
+      </c>
       <c r="B42" s="28" t="n"/>
-      <c r="C42" s="28" t="n"/>
+      <c r="C42" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D42" s="28" t="n"/>
       <c r="E42" s="28" t="n"/>
       <c r="F42" s="28" t="n"/>
@@ -19586,9 +20426,17 @@
       <c r="R42" s="28" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="28" t="n"/>
+      <c r="A43" s="28" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
       <c r="B43" s="28" t="n"/>
-      <c r="C43" s="28" t="n"/>
+      <c r="C43" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D43" s="28" t="n"/>
       <c r="E43" s="28" t="n"/>
       <c r="F43" s="28" t="n"/>
@@ -23008,9 +23856,17 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="n"/>
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-04</t>
+        </is>
+      </c>
       <c r="B35" s="29" t="n"/>
-      <c r="C35" s="28" t="n"/>
+      <c r="C35" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
@@ -23028,9 +23884,17 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="n"/>
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-11</t>
+        </is>
+      </c>
       <c r="B36" s="29" t="n"/>
-      <c r="C36" s="28" t="n"/>
+      <c r="C36" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
@@ -23048,9 +23912,17 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="n"/>
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-18</t>
+        </is>
+      </c>
       <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="n"/>
+      <c r="C37" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
@@ -23068,9 +23940,17 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="n"/>
+      <c r="A38" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-25</t>
+        </is>
+      </c>
       <c r="B38" s="28" t="n"/>
-      <c r="C38" s="28" t="n"/>
+      <c r="C38" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
@@ -23088,10 +23968,18 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="n"/>
+      <c r="A39" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-09</t>
+        </is>
+      </c>
       <c r="B39" s="28" t="n"/>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="n"/>
+      <c r="D39" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -23108,10 +23996,18 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="n"/>
+      <c r="A40" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-16</t>
+        </is>
+      </c>
       <c r="B40" s="28" t="n"/>
       <c r="C40" s="28" t="n"/>
-      <c r="D40" s="28" t="n"/>
+      <c r="D40" s="28" t="inlineStr">
+        <is>
+          <t>TP 4H</t>
+        </is>
+      </c>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
       <c r="G40" s="28" t="n"/>
@@ -24799,9 +25695,17 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="n"/>
+      <c r="A35" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-04</t>
+        </is>
+      </c>
       <c r="B35" s="29" t="n"/>
-      <c r="C35" s="28" t="n"/>
+      <c r="C35" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
@@ -24819,9 +25723,21 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="n"/>
-      <c r="B36" s="29" t="n"/>
-      <c r="C36" s="28" t="n"/>
+      <c r="A36" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-11</t>
+        </is>
+      </c>
+      <c r="B36" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C36" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
@@ -24839,9 +25755,21 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="n"/>
-      <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="n"/>
+      <c r="A37" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-18</t>
+        </is>
+      </c>
+      <c r="B37" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C37" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
@@ -24859,9 +25787,17 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="n"/>
+      <c r="A38" s="28" t="inlineStr">
+        <is>
+          <t>2023-09-25</t>
+        </is>
+      </c>
       <c r="B38" s="28" t="n"/>
-      <c r="C38" s="28" t="n"/>
+      <c r="C38" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
@@ -24879,9 +25815,17 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="n"/>
+      <c r="A39" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-09</t>
+        </is>
+      </c>
       <c r="B39" s="28" t="n"/>
-      <c r="C39" s="28" t="n"/>
+      <c r="C39" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
@@ -24899,9 +25843,17 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="n"/>
+      <c r="A40" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-16</t>
+        </is>
+      </c>
       <c r="B40" s="28" t="n"/>
-      <c r="C40" s="28" t="n"/>
+      <c r="C40" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D40" s="28" t="n"/>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
@@ -24919,9 +25871,17 @@
       <c r="R40" s="28" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="n"/>
+      <c r="A41" s="28" t="inlineStr">
+        <is>
+          <t>2023-10-23</t>
+        </is>
+      </c>
       <c r="B41" s="28" t="n"/>
-      <c r="C41" s="28" t="n"/>
+      <c r="C41" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D41" s="28" t="n"/>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
@@ -24939,10 +25899,22 @@
       <c r="R41" s="28" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="28" t="n"/>
+      <c r="A42" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
       <c r="B42" s="28" t="n"/>
-      <c r="C42" s="28" t="n"/>
-      <c r="D42" s="28" t="n"/>
+      <c r="C42" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
+      <c r="D42" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E42" s="28" t="n"/>
       <c r="F42" s="28" t="n"/>
       <c r="G42" s="28" t="n"/>
@@ -24959,10 +25931,18 @@
       <c r="R42" s="28" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="28" t="n"/>
+      <c r="A43" s="28" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
       <c r="B43" s="28" t="n"/>
       <c r="C43" s="28" t="n"/>
-      <c r="D43" s="28" t="n"/>
+      <c r="D43" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E43" s="28" t="n"/>
       <c r="F43" s="28" t="n"/>
       <c r="G43" s="28" t="n"/>

</xml_diff>

<commit_message>
changements écriture : + lisible
</commit_message>
<xml_diff>
--- a/SAE_3_01/fichiers genere/S1.xlsx
+++ b/SAE_3_01/fichiers genere/S1.xlsx
@@ -4425,7 +4425,7 @@
       </c>
       <c r="G2" s="28" t="inlineStr">
         <is>
-          <t>Josée VAQUIERI PORTOLANO</t>
+          <t>JosÃ©e VAQUIERI PORTOLANO</t>
         </is>
       </c>
       <c r="H2" s="28" t="n"/>
@@ -13870,7 +13870,7 @@
       </c>
       <c r="G2" s="28" t="inlineStr">
         <is>
-          <t>Mickaël MARTIN NEVOT</t>
+          <t>MickaÃ«l MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="28" t="n"/>
@@ -15753,7 +15753,7 @@
       </c>
       <c r="G2" s="28" t="inlineStr">
         <is>
-          <t>Mickaël MARTIN NEVOT</t>
+          <t>MickaÃ«l MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="28" t="n"/>
@@ -17588,7 +17588,7 @@
       </c>
       <c r="G2" s="28" t="inlineStr">
         <is>
-          <t>Mickaël MARTIN NEVOT</t>
+          <t>MickaÃ«l MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="28" t="n"/>
@@ -19427,7 +19427,7 @@
       </c>
       <c r="G2" s="28" t="inlineStr">
         <is>
-          <t>Mickaël MARTIN NEVOT</t>
+          <t>MickaÃ«l MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="28" t="n"/>

</xml_diff>

<commit_message>
opti + orienté objet
</commit_message>
<xml_diff>
--- a/SAE_3_01/fichiers genere/S1.xlsx
+++ b/SAE_3_01/fichiers genere/S1.xlsx
@@ -5192,7 +5192,7 @@
     <row r="36">
       <c r="A36" s="28" t="inlineStr">
         <is>
-          <t>2023-09-11</t>
+          <t>2023-09-25</t>
         </is>
       </c>
       <c r="B36" s="29" t="n"/>
@@ -5220,7 +5220,7 @@
     <row r="37">
       <c r="A37" s="28" t="inlineStr">
         <is>
-          <t>2023-09-18</t>
+          <t>2023-10-09</t>
         </is>
       </c>
       <c r="B37" s="29" t="n"/>
@@ -5248,7 +5248,7 @@
     <row r="38">
       <c r="A38" s="28" t="inlineStr">
         <is>
-          <t>2023-09-25</t>
+          <t>2023-10-16</t>
         </is>
       </c>
       <c r="B38" s="28" t="n"/>
@@ -5276,7 +5276,7 @@
     <row r="39">
       <c r="A39" s="28" t="inlineStr">
         <is>
-          <t>2023-10-09</t>
+          <t>2023-11-13</t>
         </is>
       </c>
       <c r="B39" s="28" t="n"/>
@@ -5304,7 +5304,7 @@
     <row r="40">
       <c r="A40" s="28" t="inlineStr">
         <is>
-          <t>2023-10-16</t>
+          <t>2023-11-20</t>
         </is>
       </c>
       <c r="B40" s="28" t="n"/>
@@ -5332,7 +5332,7 @@
     <row r="41">
       <c r="A41" s="28" t="inlineStr">
         <is>
-          <t>2023-10-23</t>
+          <t>2023-11-27</t>
         </is>
       </c>
       <c r="B41" s="28" t="n"/>
@@ -5360,7 +5360,7 @@
     <row r="42">
       <c r="A42" s="28" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>2023-12-04</t>
         </is>
       </c>
       <c r="B42" s="28" t="n"/>
@@ -5388,7 +5388,7 @@
     <row r="43">
       <c r="A43" s="28" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>2023-12-11</t>
         </is>
       </c>
       <c r="B43" s="28" t="n"/>
@@ -5414,18 +5414,10 @@
       <c r="R43" s="28" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-20</t>
-        </is>
-      </c>
+      <c r="A44" s="28" t="n"/>
       <c r="B44" s="28" t="n"/>
       <c r="C44" s="28" t="n"/>
-      <c r="D44" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D44" s="28" t="n"/>
       <c r="E44" s="28" t="n"/>
       <c r="F44" s="28" t="n"/>
       <c r="G44" s="28" t="n"/>
@@ -5442,18 +5434,10 @@
       <c r="R44" s="28" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-27</t>
-        </is>
-      </c>
+      <c r="A45" s="28" t="n"/>
       <c r="B45" s="28" t="n"/>
       <c r="C45" s="28" t="n"/>
-      <c r="D45" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D45" s="28" t="n"/>
       <c r="E45" s="28" t="n"/>
       <c r="F45" s="28" t="n"/>
       <c r="G45" s="28" t="n"/>
@@ -5470,18 +5454,10 @@
       <c r="R45" s="28" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-04</t>
-        </is>
-      </c>
+      <c r="A46" s="28" t="n"/>
       <c r="B46" s="28" t="n"/>
       <c r="C46" s="28" t="n"/>
-      <c r="D46" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D46" s="28" t="n"/>
       <c r="E46" s="28" t="n"/>
       <c r="F46" s="28" t="n"/>
       <c r="G46" s="28" t="n"/>
@@ -5498,18 +5474,10 @@
       <c r="R46" s="28" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-11</t>
-        </is>
-      </c>
+      <c r="A47" s="28" t="n"/>
       <c r="B47" s="28" t="n"/>
       <c r="C47" s="28" t="n"/>
-      <c r="D47" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D47" s="28" t="n"/>
       <c r="E47" s="28" t="n"/>
       <c r="F47" s="28" t="n"/>
       <c r="G47" s="28" t="n"/>
@@ -7255,7 +7223,7 @@
     <row r="42">
       <c r="A42" s="28" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>2023-11-27</t>
         </is>
       </c>
       <c r="B42" s="28" t="n"/>
@@ -7281,17 +7249,9 @@
       <c r="R42" s="28" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-20</t>
-        </is>
-      </c>
+      <c r="A43" s="28" t="n"/>
       <c r="B43" s="28" t="n"/>
-      <c r="C43" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C43" s="28" t="n"/>
       <c r="D43" s="28" t="n"/>
       <c r="E43" s="28" t="n"/>
       <c r="F43" s="28" t="n"/>
@@ -7309,17 +7269,9 @@
       <c r="R43" s="28" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-27</t>
-        </is>
-      </c>
+      <c r="A44" s="28" t="n"/>
       <c r="B44" s="28" t="n"/>
-      <c r="C44" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C44" s="28" t="n"/>
       <c r="D44" s="28" t="n"/>
       <c r="E44" s="28" t="n"/>
       <c r="F44" s="28" t="n"/>
@@ -12631,7 +12583,7 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>Amphi 4H</t>
+          <t>Amphi 2H</t>
         </is>
       </c>
       <c r="C35" s="28" t="n"/>
@@ -12659,7 +12611,7 @@
       </c>
       <c r="B36" s="29" t="inlineStr">
         <is>
-          <t>Amphi 4H</t>
+          <t>Amphi 2H</t>
         </is>
       </c>
       <c r="C36" s="28" t="inlineStr">
@@ -12803,11 +12755,7 @@
           <t>TD 2H</t>
         </is>
       </c>
-      <c r="D40" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D40" s="28" t="n"/>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
       <c r="G40" s="28" t="n"/>
@@ -12826,20 +12774,20 @@
     <row r="41">
       <c r="A41" s="28" t="inlineStr">
         <is>
-          <t>2023-10-16</t>
-        </is>
-      </c>
-      <c r="B41" s="28" t="n"/>
+          <t>2023-10-23</t>
+        </is>
+      </c>
+      <c r="B41" s="28" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
       <c r="C41" s="28" t="inlineStr">
         <is>
           <t>TD 2H</t>
         </is>
       </c>
-      <c r="D41" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D41" s="28" t="n"/>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
       <c r="G41" s="28" t="n"/>
@@ -12858,24 +12806,16 @@
     <row r="42">
       <c r="A42" s="28" t="inlineStr">
         <is>
-          <t>2023-10-23</t>
-        </is>
-      </c>
-      <c r="B42" s="28" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
+          <t>2023-11-06</t>
+        </is>
+      </c>
+      <c r="B42" s="28" t="n"/>
       <c r="C42" s="28" t="inlineStr">
         <is>
           <t>TD 2H</t>
         </is>
       </c>
-      <c r="D42" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D42" s="28" t="n"/>
       <c r="E42" s="28" t="n"/>
       <c r="F42" s="28" t="n"/>
       <c r="G42" s="28" t="n"/>
@@ -12894,20 +12834,16 @@
     <row r="43">
       <c r="A43" s="28" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
-        </is>
-      </c>
-      <c r="B43" s="28" t="n"/>
-      <c r="C43" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
-      <c r="D43" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="B43" s="28" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C43" s="28" t="n"/>
+      <c r="D43" s="28" t="n"/>
       <c r="E43" s="28" t="n"/>
       <c r="F43" s="28" t="n"/>
       <c r="G43" s="28" t="n"/>
@@ -12926,22 +12862,14 @@
     <row r="44">
       <c r="A44" s="28" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
-        </is>
-      </c>
-      <c r="B44" s="28" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
-      <c r="C44" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+          <t>2023-11-20</t>
+        </is>
+      </c>
+      <c r="B44" s="28" t="n"/>
+      <c r="C44" s="28" t="n"/>
       <c r="D44" s="28" t="inlineStr">
         <is>
-          <t>TP 6H</t>
+          <t>TP 2H</t>
         </is>
       </c>
       <c r="E44" s="28" t="n"/>
@@ -12962,10 +12890,14 @@
     <row r="45">
       <c r="A45" s="28" t="inlineStr">
         <is>
-          <t>2023-11-20</t>
-        </is>
-      </c>
-      <c r="B45" s="28" t="n"/>
+          <t>2023-11-27</t>
+        </is>
+      </c>
+      <c r="B45" s="28" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
       <c r="C45" s="28" t="inlineStr">
         <is>
           <t>TD 2H</t>
@@ -12994,22 +12926,14 @@
     <row r="46">
       <c r="A46" s="28" t="inlineStr">
         <is>
-          <t>2023-11-27</t>
-        </is>
-      </c>
-      <c r="B46" s="28" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
-      <c r="C46" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+          <t>2023-12-04</t>
+        </is>
+      </c>
+      <c r="B46" s="28" t="n"/>
+      <c r="C46" s="28" t="n"/>
       <c r="D46" s="28" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 4H</t>
         </is>
       </c>
       <c r="E46" s="28" t="n"/>
@@ -13030,7 +12954,7 @@
     <row r="47">
       <c r="A47" s="28" t="inlineStr">
         <is>
-          <t>2023-12-04</t>
+          <t>2023-12-11</t>
         </is>
       </c>
       <c r="B47" s="28" t="n"/>
@@ -13058,7 +12982,7 @@
     <row r="48">
       <c r="A48" s="28" t="inlineStr">
         <is>
-          <t>2023-12-11</t>
+          <t>2023-12-18</t>
         </is>
       </c>
       <c r="B48" s="28" t="n"/>
@@ -13086,16 +13010,12 @@
     <row r="49">
       <c r="A49" s="28" t="inlineStr">
         <is>
-          <t>2023-12-18</t>
+          <t>2024-01-08</t>
         </is>
       </c>
       <c r="B49" s="28" t="n"/>
       <c r="C49" s="28" t="n"/>
-      <c r="D49" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D49" s="28" t="n"/>
       <c r="E49" s="28" t="n"/>
       <c r="F49" s="28" t="n"/>
       <c r="G49" s="28" t="n"/>
@@ -13112,11 +13032,7 @@
       <c r="R49" s="28" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="28" t="inlineStr">
-        <is>
-          <t>2024-01-08</t>
-        </is>
-      </c>
+      <c r="A50" s="28" t="n"/>
       <c r="B50" s="28" t="n"/>
       <c r="C50" s="28" t="n"/>
       <c r="D50" s="28" t="n"/>
@@ -16492,15 +16408,15 @@
     <row r="35">
       <c r="A35" s="28" t="inlineStr">
         <is>
-          <t>2023-09-18</t>
-        </is>
-      </c>
-      <c r="B35" s="29" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
-      <c r="C35" s="28" t="n"/>
+          <t>2023-10-02</t>
+        </is>
+      </c>
+      <c r="B35" s="29" t="n"/>
+      <c r="C35" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
@@ -16520,16 +16436,16 @@
     <row r="36">
       <c r="A36" s="28" t="inlineStr">
         <is>
-          <t>2023-09-25</t>
-        </is>
-      </c>
-      <c r="B36" s="29" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
+          <t>2023-10-09</t>
+        </is>
+      </c>
+      <c r="B36" s="29" t="n"/>
       <c r="C36" s="28" t="n"/>
-      <c r="D36" s="28" t="n"/>
+      <c r="D36" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
       <c r="G36" s="28" t="n"/>
@@ -16548,16 +16464,16 @@
     <row r="37">
       <c r="A37" s="28" t="inlineStr">
         <is>
-          <t>2023-10-02</t>
+          <t>2023-10-16</t>
         </is>
       </c>
       <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
-      <c r="D37" s="28" t="n"/>
+      <c r="C37" s="28" t="n"/>
+      <c r="D37" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
       <c r="G37" s="28" t="n"/>
@@ -16576,16 +16492,12 @@
     <row r="38">
       <c r="A38" s="28" t="inlineStr">
         <is>
-          <t>2023-10-09</t>
+          <t>2023-10-23</t>
         </is>
       </c>
       <c r="B38" s="28" t="n"/>
       <c r="C38" s="28" t="n"/>
-      <c r="D38" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
       <c r="G38" s="28" t="n"/>
@@ -16602,18 +16514,10 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-16</t>
-        </is>
-      </c>
+      <c r="A39" s="28" t="n"/>
       <c r="B39" s="28" t="n"/>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -16630,11 +16534,7 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-23</t>
-        </is>
-      </c>
+      <c r="A40" s="28" t="n"/>
       <c r="B40" s="28" t="n"/>
       <c r="C40" s="28" t="n"/>
       <c r="D40" s="28" t="n"/>
@@ -18330,11 +18230,7 @@
           <t>2023-09-04</t>
         </is>
       </c>
-      <c r="B35" s="29" t="inlineStr">
-        <is>
-          <t>Amphi 4H</t>
-        </is>
-      </c>
+      <c r="B35" s="29" t="n"/>
       <c r="C35" s="28" t="n"/>
       <c r="D35" s="28" t="inlineStr">
         <is>
@@ -18362,11 +18258,7 @@
           <t>2023-09-11</t>
         </is>
       </c>
-      <c r="B36" s="29" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
+      <c r="B36" s="29" t="n"/>
       <c r="C36" s="28" t="n"/>
       <c r="D36" s="28" t="inlineStr">
         <is>
@@ -18426,7 +18318,7 @@
       <c r="C38" s="28" t="n"/>
       <c r="D38" s="28" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H</t>
         </is>
       </c>
       <c r="E38" s="28" t="n"/>
@@ -20315,11 +20207,7 @@
           <t>2023-11-13</t>
         </is>
       </c>
-      <c r="B39" s="28" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
+      <c r="B39" s="28" t="n"/>
       <c r="C39" s="28" t="n"/>
       <c r="D39" s="28" t="inlineStr">
         <is>
@@ -20432,11 +20320,7 @@
         </is>
       </c>
       <c r="B43" s="28" t="n"/>
-      <c r="C43" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
+      <c r="C43" s="28" t="n"/>
       <c r="D43" s="28" t="n"/>
       <c r="E43" s="28" t="n"/>
       <c r="F43" s="28" t="n"/>
@@ -23948,7 +23832,7 @@
       <c r="B38" s="28" t="n"/>
       <c r="C38" s="28" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H</t>
         </is>
       </c>
       <c r="D38" s="28" t="n"/>
@@ -23977,7 +23861,7 @@
       <c r="C39" s="28" t="n"/>
       <c r="D39" s="28" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H</t>
         </is>
       </c>
       <c r="E39" s="28" t="n"/>
@@ -25697,15 +25581,15 @@
     <row r="35">
       <c r="A35" s="28" t="inlineStr">
         <is>
-          <t>2023-09-04</t>
-        </is>
-      </c>
-      <c r="B35" s="29" t="n"/>
-      <c r="C35" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+          <t>2023-09-11</t>
+        </is>
+      </c>
+      <c r="B35" s="29" t="inlineStr">
+        <is>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C35" s="28" t="n"/>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
@@ -25725,7 +25609,7 @@
     <row r="36">
       <c r="A36" s="28" t="inlineStr">
         <is>
-          <t>2023-09-11</t>
+          <t>2023-09-18</t>
         </is>
       </c>
       <c r="B36" s="29" t="inlineStr">
@@ -25757,14 +25641,10 @@
     <row r="37">
       <c r="A37" s="28" t="inlineStr">
         <is>
-          <t>2023-09-18</t>
-        </is>
-      </c>
-      <c r="B37" s="29" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
+          <t>2023-10-23</t>
+        </is>
+      </c>
+      <c r="B37" s="29" t="n"/>
       <c r="C37" s="28" t="inlineStr">
         <is>
           <t>TD 2H</t>
@@ -25789,7 +25669,7 @@
     <row r="38">
       <c r="A38" s="28" t="inlineStr">
         <is>
-          <t>2023-09-25</t>
+          <t>2023-11-06</t>
         </is>
       </c>
       <c r="B38" s="28" t="n"/>
@@ -25798,7 +25678,11 @@
           <t>TD 2H</t>
         </is>
       </c>
-      <c r="D38" s="28" t="n"/>
+      <c r="D38" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
       <c r="G38" s="28" t="n"/>
@@ -25817,16 +25701,16 @@
     <row r="39">
       <c r="A39" s="28" t="inlineStr">
         <is>
-          <t>2023-10-09</t>
+          <t>2023-11-13</t>
         </is>
       </c>
       <c r="B39" s="28" t="n"/>
-      <c r="C39" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
-      <c r="D39" s="28" t="n"/>
+      <c r="C39" s="28" t="n"/>
+      <c r="D39" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -25843,17 +25727,9 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-16</t>
-        </is>
-      </c>
+      <c r="A40" s="28" t="n"/>
       <c r="B40" s="28" t="n"/>
-      <c r="C40" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C40" s="28" t="n"/>
       <c r="D40" s="28" t="n"/>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
@@ -25871,17 +25747,9 @@
       <c r="R40" s="28" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-23</t>
-        </is>
-      </c>
+      <c r="A41" s="28" t="n"/>
       <c r="B41" s="28" t="n"/>
-      <c r="C41" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
+      <c r="C41" s="28" t="n"/>
       <c r="D41" s="28" t="n"/>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
@@ -25899,22 +25767,10 @@
       <c r="R41" s="28" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-06</t>
-        </is>
-      </c>
+      <c r="A42" s="28" t="n"/>
       <c r="B42" s="28" t="n"/>
-      <c r="C42" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
-      <c r="D42" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="C42" s="28" t="n"/>
+      <c r="D42" s="28" t="n"/>
       <c r="E42" s="28" t="n"/>
       <c r="F42" s="28" t="n"/>
       <c r="G42" s="28" t="n"/>
@@ -25931,18 +25787,10 @@
       <c r="R42" s="28" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-13</t>
-        </is>
-      </c>
+      <c r="A43" s="28" t="n"/>
       <c r="B43" s="28" t="n"/>
       <c r="C43" s="28" t="n"/>
-      <c r="D43" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D43" s="28" t="n"/>
       <c r="E43" s="28" t="n"/>
       <c r="F43" s="28" t="n"/>
       <c r="G43" s="28" t="n"/>

</xml_diff>

<commit_message>
ajout du nombre d'erreurs total + renomage fichier rapport erreur
</commit_message>
<xml_diff>
--- a/SAE_3_01/fichiers genere/S1.xlsx
+++ b/SAE_3_01/fichiers genere/S1.xlsx
@@ -3341,16 +3341,16 @@
     <row r="36">
       <c r="A36" s="28" t="inlineStr">
         <is>
-          <t>2023-11-20</t>
+          <t>2024-01-08</t>
         </is>
       </c>
       <c r="B36" s="29" t="n"/>
-      <c r="C36" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
-      <c r="D36" s="28" t="n"/>
+      <c r="C36" s="28" t="n"/>
+      <c r="D36" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
       <c r="G36" s="28" t="n"/>
@@ -3367,17 +3367,9 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-27</t>
-        </is>
-      </c>
+      <c r="A37" s="28" t="n"/>
       <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C37" s="28" t="n"/>
       <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
@@ -3395,17 +3387,9 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-04</t>
-        </is>
-      </c>
+      <c r="A38" s="28" t="n"/>
       <c r="B38" s="28" t="n"/>
-      <c r="C38" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C38" s="28" t="n"/>
       <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
@@ -3423,17 +3407,9 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-11</t>
-        </is>
-      </c>
+      <c r="A39" s="28" t="n"/>
       <c r="B39" s="28" t="n"/>
-      <c r="C39" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
+      <c r="C39" s="28" t="n"/>
       <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
@@ -3451,17 +3427,9 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-18</t>
-        </is>
-      </c>
+      <c r="A40" s="28" t="n"/>
       <c r="B40" s="28" t="n"/>
-      <c r="C40" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C40" s="28" t="n"/>
       <c r="D40" s="28" t="n"/>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
@@ -3479,22 +3447,10 @@
       <c r="R40" s="28" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="inlineStr">
-        <is>
-          <t>2024-01-08</t>
-        </is>
-      </c>
+      <c r="A41" s="28" t="n"/>
       <c r="B41" s="28" t="n"/>
-      <c r="C41" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
-      <c r="D41" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="C41" s="28" t="n"/>
+      <c r="D41" s="28" t="n"/>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
       <c r="G41" s="28" t="n"/>
@@ -5164,7 +5120,7 @@
     <row r="35">
       <c r="A35" s="28" t="inlineStr">
         <is>
-          <t>2023-09-04</t>
+          <t>2023-11-20</t>
         </is>
       </c>
       <c r="B35" s="29" t="n"/>
@@ -5190,18 +5146,10 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="inlineStr">
-        <is>
-          <t>2023-09-25</t>
-        </is>
-      </c>
+      <c r="A36" s="28" t="n"/>
       <c r="B36" s="29" t="n"/>
       <c r="C36" s="28" t="n"/>
-      <c r="D36" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
       <c r="G36" s="28" t="n"/>
@@ -5218,18 +5166,10 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-09</t>
-        </is>
-      </c>
+      <c r="A37" s="28" t="n"/>
       <c r="B37" s="29" t="n"/>
       <c r="C37" s="28" t="n"/>
-      <c r="D37" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
       <c r="G37" s="28" t="n"/>
@@ -5246,18 +5186,10 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-16</t>
-        </is>
-      </c>
+      <c r="A38" s="28" t="n"/>
       <c r="B38" s="28" t="n"/>
       <c r="C38" s="28" t="n"/>
-      <c r="D38" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
       <c r="G38" s="28" t="n"/>
@@ -5274,18 +5206,10 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-13</t>
-        </is>
-      </c>
+      <c r="A39" s="28" t="n"/>
       <c r="B39" s="28" t="n"/>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -5302,18 +5226,10 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-20</t>
-        </is>
-      </c>
+      <c r="A40" s="28" t="n"/>
       <c r="B40" s="28" t="n"/>
       <c r="C40" s="28" t="n"/>
-      <c r="D40" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D40" s="28" t="n"/>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
       <c r="G40" s="28" t="n"/>
@@ -5330,18 +5246,10 @@
       <c r="R40" s="28" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-27</t>
-        </is>
-      </c>
+      <c r="A41" s="28" t="n"/>
       <c r="B41" s="28" t="n"/>
       <c r="C41" s="28" t="n"/>
-      <c r="D41" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D41" s="28" t="n"/>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
       <c r="G41" s="28" t="n"/>
@@ -5358,18 +5266,10 @@
       <c r="R41" s="28" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-04</t>
-        </is>
-      </c>
+      <c r="A42" s="28" t="n"/>
       <c r="B42" s="28" t="n"/>
       <c r="C42" s="28" t="n"/>
-      <c r="D42" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D42" s="28" t="n"/>
       <c r="E42" s="28" t="n"/>
       <c r="F42" s="28" t="n"/>
       <c r="G42" s="28" t="n"/>
@@ -5386,18 +5286,10 @@
       <c r="R42" s="28" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-11</t>
-        </is>
-      </c>
+      <c r="A43" s="28" t="n"/>
       <c r="B43" s="28" t="n"/>
       <c r="C43" s="28" t="n"/>
-      <c r="D43" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D43" s="28" t="n"/>
       <c r="E43" s="28" t="n"/>
       <c r="F43" s="28" t="n"/>
       <c r="G43" s="28" t="n"/>
@@ -7027,7 +6919,7 @@
     <row r="35">
       <c r="A35" s="28" t="inlineStr">
         <is>
-          <t>2023-09-11</t>
+          <t>2023-11-06</t>
         </is>
       </c>
       <c r="B35" s="29" t="n"/>
@@ -7053,17 +6945,9 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="inlineStr">
-        <is>
-          <t>2023-09-18</t>
-        </is>
-      </c>
+      <c r="A36" s="28" t="n"/>
       <c r="B36" s="29" t="n"/>
-      <c r="C36" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C36" s="28" t="n"/>
       <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
@@ -7081,17 +6965,9 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="inlineStr">
-        <is>
-          <t>2023-09-25</t>
-        </is>
-      </c>
+      <c r="A37" s="28" t="n"/>
       <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C37" s="28" t="n"/>
       <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
@@ -7109,17 +6985,9 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-09</t>
-        </is>
-      </c>
+      <c r="A38" s="28" t="n"/>
       <c r="B38" s="28" t="n"/>
-      <c r="C38" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C38" s="28" t="n"/>
       <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
@@ -7137,17 +7005,9 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-16</t>
-        </is>
-      </c>
+      <c r="A39" s="28" t="n"/>
       <c r="B39" s="28" t="n"/>
-      <c r="C39" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C39" s="28" t="n"/>
       <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
@@ -7165,17 +7025,9 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-23</t>
-        </is>
-      </c>
+      <c r="A40" s="28" t="n"/>
       <c r="B40" s="28" t="n"/>
-      <c r="C40" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C40" s="28" t="n"/>
       <c r="D40" s="28" t="n"/>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
@@ -7193,17 +7045,9 @@
       <c r="R40" s="28" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-06</t>
-        </is>
-      </c>
+      <c r="A41" s="28" t="n"/>
       <c r="B41" s="28" t="n"/>
-      <c r="C41" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C41" s="28" t="n"/>
       <c r="D41" s="28" t="n"/>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
@@ -7221,17 +7065,9 @@
       <c r="R41" s="28" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-27</t>
-        </is>
-      </c>
+      <c r="A42" s="28" t="n"/>
       <c r="B42" s="28" t="n"/>
-      <c r="C42" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C42" s="28" t="n"/>
       <c r="D42" s="28" t="n"/>
       <c r="E42" s="28" t="n"/>
       <c r="F42" s="28" t="n"/>
@@ -8882,16 +8718,16 @@
     <row r="35">
       <c r="A35" s="28" t="inlineStr">
         <is>
-          <t>2023-11-27</t>
+          <t>2024-01-08</t>
         </is>
       </c>
       <c r="B35" s="29" t="n"/>
-      <c r="C35" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
-      <c r="D35" s="28" t="n"/>
+      <c r="C35" s="28" t="n"/>
+      <c r="D35" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
       <c r="G35" s="28" t="n"/>
@@ -8908,17 +8744,9 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-04</t>
-        </is>
-      </c>
+      <c r="A36" s="28" t="n"/>
       <c r="B36" s="29" t="n"/>
-      <c r="C36" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C36" s="28" t="n"/>
       <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
@@ -8936,17 +8764,9 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-11</t>
-        </is>
-      </c>
+      <c r="A37" s="28" t="n"/>
       <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C37" s="28" t="n"/>
       <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
@@ -8964,17 +8784,9 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-18</t>
-        </is>
-      </c>
+      <c r="A38" s="28" t="n"/>
       <c r="B38" s="28" t="n"/>
-      <c r="C38" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C38" s="28" t="n"/>
       <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
@@ -8992,18 +8804,10 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="inlineStr">
-        <is>
-          <t>2024-01-08</t>
-        </is>
-      </c>
+      <c r="A39" s="28" t="n"/>
       <c r="B39" s="28" t="n"/>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -12578,15 +12382,19 @@
     <row r="35">
       <c r="A35" s="28" t="inlineStr">
         <is>
-          <t>2023-09-04</t>
+          <t>2023-09-18</t>
         </is>
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
-      <c r="C35" s="28" t="n"/>
+          <t>Amphi 4H</t>
+        </is>
+      </c>
+      <c r="C35" s="28" t="inlineStr">
+        <is>
+          <t>TD 2H</t>
+        </is>
+      </c>
       <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
@@ -12606,7 +12414,7 @@
     <row r="36">
       <c r="A36" s="28" t="inlineStr">
         <is>
-          <t>2023-09-11</t>
+          <t>2023-09-25</t>
         </is>
       </c>
       <c r="B36" s="29" t="inlineStr">
@@ -12638,19 +12446,15 @@
     <row r="37">
       <c r="A37" s="28" t="inlineStr">
         <is>
-          <t>2023-09-18</t>
+          <t>2023-10-02</t>
         </is>
       </c>
       <c r="B37" s="29" t="inlineStr">
         <is>
-          <t>Amphi 4H</t>
-        </is>
-      </c>
-      <c r="C37" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
+          <t>Amphi 2H</t>
+        </is>
+      </c>
+      <c r="C37" s="28" t="n"/>
       <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
@@ -12670,24 +12474,12 @@
     <row r="38">
       <c r="A38" s="28" t="inlineStr">
         <is>
-          <t>2023-09-25</t>
-        </is>
-      </c>
-      <c r="B38" s="28" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
-      <c r="C38" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
-      <c r="D38" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+          <t>2023-10-09</t>
+        </is>
+      </c>
+      <c r="B38" s="28" t="n"/>
+      <c r="C38" s="28" t="n"/>
+      <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
       <c r="G38" s="28" t="n"/>
@@ -12706,7 +12498,7 @@
     <row r="39">
       <c r="A39" s="28" t="inlineStr">
         <is>
-          <t>2023-10-02</t>
+          <t>2023-10-23</t>
         </is>
       </c>
       <c r="B39" s="28" t="inlineStr">
@@ -12714,16 +12506,8 @@
           <t>Amphi 2H</t>
         </is>
       </c>
-      <c r="C39" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
-      <c r="D39" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="C39" s="28" t="n"/>
+      <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -12742,7 +12526,7 @@
     <row r="40">
       <c r="A40" s="28" t="inlineStr">
         <is>
-          <t>2023-10-09</t>
+          <t>2023-11-13</t>
         </is>
       </c>
       <c r="B40" s="28" t="inlineStr">
@@ -12750,11 +12534,7 @@
           <t>Amphi 2H</t>
         </is>
       </c>
-      <c r="C40" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C40" s="28" t="n"/>
       <c r="D40" s="28" t="n"/>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
@@ -12774,20 +12554,16 @@
     <row r="41">
       <c r="A41" s="28" t="inlineStr">
         <is>
-          <t>2023-10-23</t>
-        </is>
-      </c>
-      <c r="B41" s="28" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
-      <c r="C41" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
-      <c r="D41" s="28" t="n"/>
+          <t>2023-11-20</t>
+        </is>
+      </c>
+      <c r="B41" s="28" t="n"/>
+      <c r="C41" s="28" t="n"/>
+      <c r="D41" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
       <c r="G41" s="28" t="n"/>
@@ -12806,7 +12582,7 @@
     <row r="42">
       <c r="A42" s="28" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>2023-11-27</t>
         </is>
       </c>
       <c r="B42" s="28" t="n"/>
@@ -12815,7 +12591,11 @@
           <t>TD 2H</t>
         </is>
       </c>
-      <c r="D42" s="28" t="n"/>
+      <c r="D42" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E42" s="28" t="n"/>
       <c r="F42" s="28" t="n"/>
       <c r="G42" s="28" t="n"/>
@@ -12834,16 +12614,16 @@
     <row r="43">
       <c r="A43" s="28" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
-        </is>
-      </c>
-      <c r="B43" s="28" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
+          <t>2023-12-04</t>
+        </is>
+      </c>
+      <c r="B43" s="28" t="n"/>
       <c r="C43" s="28" t="n"/>
-      <c r="D43" s="28" t="n"/>
+      <c r="D43" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E43" s="28" t="n"/>
       <c r="F43" s="28" t="n"/>
       <c r="G43" s="28" t="n"/>
@@ -12862,16 +12642,12 @@
     <row r="44">
       <c r="A44" s="28" t="inlineStr">
         <is>
-          <t>2023-11-20</t>
+          <t>2024-01-08</t>
         </is>
       </c>
       <c r="B44" s="28" t="n"/>
       <c r="C44" s="28" t="n"/>
-      <c r="D44" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D44" s="28" t="n"/>
       <c r="E44" s="28" t="n"/>
       <c r="F44" s="28" t="n"/>
       <c r="G44" s="28" t="n"/>
@@ -12888,26 +12664,10 @@
       <c r="R44" s="28" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-27</t>
-        </is>
-      </c>
-      <c r="B45" s="28" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
-      <c r="C45" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
-      <c r="D45" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="A45" s="28" t="n"/>
+      <c r="B45" s="28" t="n"/>
+      <c r="C45" s="28" t="n"/>
+      <c r="D45" s="28" t="n"/>
       <c r="E45" s="28" t="n"/>
       <c r="F45" s="28" t="n"/>
       <c r="G45" s="28" t="n"/>
@@ -12924,18 +12684,10 @@
       <c r="R45" s="28" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-04</t>
-        </is>
-      </c>
+      <c r="A46" s="28" t="n"/>
       <c r="B46" s="28" t="n"/>
       <c r="C46" s="28" t="n"/>
-      <c r="D46" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D46" s="28" t="n"/>
       <c r="E46" s="28" t="n"/>
       <c r="F46" s="28" t="n"/>
       <c r="G46" s="28" t="n"/>
@@ -12952,18 +12704,10 @@
       <c r="R46" s="28" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-11</t>
-        </is>
-      </c>
+      <c r="A47" s="28" t="n"/>
       <c r="B47" s="28" t="n"/>
       <c r="C47" s="28" t="n"/>
-      <c r="D47" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D47" s="28" t="n"/>
       <c r="E47" s="28" t="n"/>
       <c r="F47" s="28" t="n"/>
       <c r="G47" s="28" t="n"/>
@@ -12980,18 +12724,10 @@
       <c r="R47" s="28" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-18</t>
-        </is>
-      </c>
+      <c r="A48" s="28" t="n"/>
       <c r="B48" s="28" t="n"/>
       <c r="C48" s="28" t="n"/>
-      <c r="D48" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D48" s="28" t="n"/>
       <c r="E48" s="28" t="n"/>
       <c r="F48" s="28" t="n"/>
       <c r="G48" s="28" t="n"/>
@@ -13008,11 +12744,7 @@
       <c r="R48" s="28" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="28" t="inlineStr">
-        <is>
-          <t>2024-01-08</t>
-        </is>
-      </c>
+      <c r="A49" s="28" t="n"/>
       <c r="B49" s="28" t="n"/>
       <c r="C49" s="28" t="n"/>
       <c r="D49" s="28" t="n"/>
@@ -14610,11 +14342,7 @@
         </is>
       </c>
       <c r="C36" s="28" t="n"/>
-      <c r="D36" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
       <c r="G36" s="28" t="n"/>
@@ -14668,7 +14396,7 @@
       <c r="C38" s="28" t="n"/>
       <c r="D38" s="28" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H</t>
         </is>
       </c>
       <c r="E38" s="28" t="n"/>
@@ -16408,16 +16136,16 @@
     <row r="35">
       <c r="A35" s="28" t="inlineStr">
         <is>
-          <t>2023-10-02</t>
+          <t>2023-10-09</t>
         </is>
       </c>
       <c r="B35" s="29" t="n"/>
-      <c r="C35" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
-      <c r="D35" s="28" t="n"/>
+      <c r="C35" s="28" t="n"/>
+      <c r="D35" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
       <c r="G35" s="28" t="n"/>
@@ -16436,16 +16164,12 @@
     <row r="36">
       <c r="A36" s="28" t="inlineStr">
         <is>
-          <t>2023-10-09</t>
+          <t>2023-10-23</t>
         </is>
       </c>
       <c r="B36" s="29" t="n"/>
       <c r="C36" s="28" t="n"/>
-      <c r="D36" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
       <c r="G36" s="28" t="n"/>
@@ -16462,18 +16186,10 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-16</t>
-        </is>
-      </c>
+      <c r="A37" s="28" t="n"/>
       <c r="B37" s="29" t="n"/>
       <c r="C37" s="28" t="n"/>
-      <c r="D37" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
       <c r="G37" s="28" t="n"/>
@@ -16490,11 +16206,7 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-23</t>
-        </is>
-      </c>
+      <c r="A38" s="28" t="n"/>
       <c r="B38" s="28" t="n"/>
       <c r="C38" s="28" t="n"/>
       <c r="D38" s="28" t="n"/>
@@ -18225,18 +17937,10 @@
       <c r="R34" s="28" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="inlineStr">
-        <is>
-          <t>2023-09-04</t>
-        </is>
-      </c>
+      <c r="A35" s="28" t="n"/>
       <c r="B35" s="29" t="n"/>
       <c r="C35" s="28" t="n"/>
-      <c r="D35" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D35" s="28" t="n"/>
       <c r="E35" s="28" t="n"/>
       <c r="F35" s="28" t="n"/>
       <c r="G35" s="28" t="n"/>
@@ -18253,18 +17957,10 @@
       <c r="R35" s="28" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="28" t="inlineStr">
-        <is>
-          <t>2023-09-11</t>
-        </is>
-      </c>
+      <c r="A36" s="28" t="n"/>
       <c r="B36" s="29" t="n"/>
       <c r="C36" s="28" t="n"/>
-      <c r="D36" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
       <c r="G36" s="28" t="n"/>
@@ -18281,18 +17977,10 @@
       <c r="R36" s="28" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="28" t="inlineStr">
-        <is>
-          <t>2023-09-18</t>
-        </is>
-      </c>
+      <c r="A37" s="28" t="n"/>
       <c r="B37" s="29" t="n"/>
       <c r="C37" s="28" t="n"/>
-      <c r="D37" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D37" s="28" t="n"/>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
       <c r="G37" s="28" t="n"/>
@@ -18309,18 +17997,10 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="inlineStr">
-        <is>
-          <t>2023-09-25</t>
-        </is>
-      </c>
+      <c r="A38" s="28" t="n"/>
       <c r="B38" s="28" t="n"/>
       <c r="C38" s="28" t="n"/>
-      <c r="D38" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
       <c r="G38" s="28" t="n"/>
@@ -18337,17 +18017,9 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-02</t>
-        </is>
-      </c>
+      <c r="A39" s="28" t="n"/>
       <c r="B39" s="28" t="n"/>
-      <c r="C39" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
+      <c r="C39" s="28" t="n"/>
       <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
@@ -20084,7 +19756,7 @@
     <row r="35">
       <c r="A35" s="28" t="inlineStr">
         <is>
-          <t>2023-10-09</t>
+          <t>2023-10-16</t>
         </is>
       </c>
       <c r="B35" s="29" t="inlineStr">
@@ -20112,7 +19784,7 @@
     <row r="36">
       <c r="A36" s="28" t="inlineStr">
         <is>
-          <t>2023-10-16</t>
+          <t>2023-10-23</t>
         </is>
       </c>
       <c r="B36" s="29" t="inlineStr">
@@ -20140,7 +19812,7 @@
     <row r="37">
       <c r="A37" s="28" t="inlineStr">
         <is>
-          <t>2023-10-23</t>
+          <t>2023-11-06</t>
         </is>
       </c>
       <c r="B37" s="29" t="inlineStr">
@@ -20151,7 +19823,7 @@
       <c r="C37" s="28" t="n"/>
       <c r="D37" s="28" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H</t>
         </is>
       </c>
       <c r="E37" s="28" t="n"/>
@@ -20172,18 +19844,14 @@
     <row r="38">
       <c r="A38" s="28" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
-        </is>
-      </c>
-      <c r="B38" s="28" t="inlineStr">
-        <is>
-          <t>Amphi 2H</t>
-        </is>
-      </c>
+          <t>2023-11-27</t>
+        </is>
+      </c>
+      <c r="B38" s="28" t="n"/>
       <c r="C38" s="28" t="n"/>
       <c r="D38" s="28" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H</t>
         </is>
       </c>
       <c r="E38" s="28" t="n"/>
@@ -20204,16 +19872,16 @@
     <row r="39">
       <c r="A39" s="28" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>2023-12-04</t>
         </is>
       </c>
       <c r="B39" s="28" t="n"/>
-      <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="C39" s="28" t="inlineStr">
+        <is>
+          <t>TD 4H</t>
+        </is>
+      </c>
+      <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -20232,16 +19900,12 @@
     <row r="40">
       <c r="A40" s="28" t="inlineStr">
         <is>
-          <t>2023-11-27</t>
+          <t>2023-12-18</t>
         </is>
       </c>
       <c r="B40" s="28" t="n"/>
       <c r="C40" s="28" t="n"/>
-      <c r="D40" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D40" s="28" t="n"/>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
       <c r="G40" s="28" t="n"/>
@@ -20258,17 +19922,9 @@
       <c r="R40" s="28" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-04</t>
-        </is>
-      </c>
+      <c r="A41" s="28" t="n"/>
       <c r="B41" s="28" t="n"/>
-      <c r="C41" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
+      <c r="C41" s="28" t="n"/>
       <c r="D41" s="28" t="n"/>
       <c r="E41" s="28" t="n"/>
       <c r="F41" s="28" t="n"/>
@@ -20286,17 +19942,9 @@
       <c r="R41" s="28" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-11</t>
-        </is>
-      </c>
+      <c r="A42" s="28" t="n"/>
       <c r="B42" s="28" t="n"/>
-      <c r="C42" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
+      <c r="C42" s="28" t="n"/>
       <c r="D42" s="28" t="n"/>
       <c r="E42" s="28" t="n"/>
       <c r="F42" s="28" t="n"/>
@@ -20314,11 +19962,7 @@
       <c r="R42" s="28" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="28" t="inlineStr">
-        <is>
-          <t>2023-12-18</t>
-        </is>
-      </c>
+      <c r="A43" s="28" t="n"/>
       <c r="B43" s="28" t="n"/>
       <c r="C43" s="28" t="n"/>
       <c r="D43" s="28" t="n"/>
@@ -23748,7 +23392,7 @@
       <c r="B35" s="29" t="n"/>
       <c r="C35" s="28" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H</t>
         </is>
       </c>
       <c r="D35" s="28" t="n"/>
@@ -23770,13 +23414,13 @@
     <row r="36">
       <c r="A36" s="28" t="inlineStr">
         <is>
-          <t>2023-09-11</t>
+          <t>2023-09-25</t>
         </is>
       </c>
       <c r="B36" s="29" t="n"/>
       <c r="C36" s="28" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H</t>
         </is>
       </c>
       <c r="D36" s="28" t="n"/>
@@ -23798,16 +23442,16 @@
     <row r="37">
       <c r="A37" s="28" t="inlineStr">
         <is>
-          <t>2023-09-18</t>
+          <t>2023-10-16</t>
         </is>
       </c>
       <c r="B37" s="29" t="n"/>
-      <c r="C37" s="28" t="inlineStr">
-        <is>
-          <t>TD 4H</t>
-        </is>
-      </c>
-      <c r="D37" s="28" t="n"/>
+      <c r="C37" s="28" t="n"/>
+      <c r="D37" s="28" t="inlineStr">
+        <is>
+          <t>TP 2H</t>
+        </is>
+      </c>
       <c r="E37" s="28" t="n"/>
       <c r="F37" s="28" t="n"/>
       <c r="G37" s="28" t="n"/>
@@ -23824,17 +23468,9 @@
       <c r="R37" s="28" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="28" t="inlineStr">
-        <is>
-          <t>2023-09-25</t>
-        </is>
-      </c>
+      <c r="A38" s="28" t="n"/>
       <c r="B38" s="28" t="n"/>
-      <c r="C38" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C38" s="28" t="n"/>
       <c r="D38" s="28" t="n"/>
       <c r="E38" s="28" t="n"/>
       <c r="F38" s="28" t="n"/>
@@ -23852,18 +23488,10 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-09</t>
-        </is>
-      </c>
+      <c r="A39" s="28" t="n"/>
       <c r="B39" s="28" t="n"/>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>
@@ -23880,18 +23508,10 @@
       <c r="R39" s="28" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="28" t="inlineStr">
-        <is>
-          <t>2023-10-16</t>
-        </is>
-      </c>
+      <c r="A40" s="28" t="n"/>
       <c r="B40" s="28" t="n"/>
       <c r="C40" s="28" t="n"/>
-      <c r="D40" s="28" t="inlineStr">
-        <is>
-          <t>TP 4H</t>
-        </is>
-      </c>
+      <c r="D40" s="28" t="n"/>
       <c r="E40" s="28" t="n"/>
       <c r="F40" s="28" t="n"/>
       <c r="G40" s="28" t="n"/>
@@ -25617,11 +25237,7 @@
           <t>Amphi 2H</t>
         </is>
       </c>
-      <c r="C36" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C36" s="28" t="n"/>
       <c r="D36" s="28" t="n"/>
       <c r="E36" s="28" t="n"/>
       <c r="F36" s="28" t="n"/>
@@ -25641,7 +25257,7 @@
     <row r="37">
       <c r="A37" s="28" t="inlineStr">
         <is>
-          <t>2023-10-23</t>
+          <t>2023-11-06</t>
         </is>
       </c>
       <c r="B37" s="29" t="n"/>
@@ -25669,15 +25285,11 @@
     <row r="38">
       <c r="A38" s="28" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>2023-11-13</t>
         </is>
       </c>
       <c r="B38" s="28" t="n"/>
-      <c r="C38" s="28" t="inlineStr">
-        <is>
-          <t>TD 2H</t>
-        </is>
-      </c>
+      <c r="C38" s="28" t="n"/>
       <c r="D38" s="28" t="inlineStr">
         <is>
           <t>TP 2H</t>
@@ -25699,18 +25311,10 @@
       <c r="R38" s="28" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="28" t="inlineStr">
-        <is>
-          <t>2023-11-13</t>
-        </is>
-      </c>
+      <c r="A39" s="28" t="n"/>
       <c r="B39" s="28" t="n"/>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="28" t="inlineStr">
-        <is>
-          <t>TP 2H</t>
-        </is>
-      </c>
+      <c r="D39" s="28" t="n"/>
       <c r="E39" s="28" t="n"/>
       <c r="F39" s="28" t="n"/>
       <c r="G39" s="28" t="n"/>

</xml_diff>

<commit_message>
correction de bugs, ajout des salles, facilité
</commit_message>
<xml_diff>
--- a/SAE_3_01/fichiers genere/S1.xlsx
+++ b/SAE_3_01/fichiers genere/S1.xlsx
@@ -7,18 +7,18 @@
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="R1.01 Initiation au développeme" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="R1.02 Développement d'interface" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="R1.03 Introduction à l'architec" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="R1.04 Introduction aux systèmes" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="R1.05 Introduction aux bases de" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="R1.07 Outils mathématiques fond" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="R1.08 Introduction à la gestion" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="R1.09 Introduction à l'économie" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="R1.01 Initiation au développement" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="R1.02 Développement d'interfaces web" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="R1.03 Introduction à l'architecture des ordinateurs" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="R1.04 Introduction aux systèmes d'exploitation, à leur fonctionnement" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="R1.05 Introduction aux bases de données et SQL" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="R1.07 Outils mathématiques fondamentaux" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="R1.08 Introduction à la gestion des organisations" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="R1.09 Introduction à l'économie durable et numérique" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="R1.10 Anglais technique" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="R1.11 Bases de la communication" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="R1.12 PPP" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="R1.L.1 Méthodologie du travail " sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="R1.L.1 Méthodologie du travail universitaire" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
@@ -3283,7 +3283,7 @@
       <c r="C35" s="27" t="n"/>
       <c r="D35" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E35" s="27" t="n"/>
@@ -3311,7 +3311,7 @@
       <c r="C36" s="27" t="n"/>
       <c r="D36" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E36" s="27" t="n"/>
@@ -3339,7 +3339,7 @@
       <c r="C37" s="27" t="n"/>
       <c r="D37" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E37" s="27" t="n"/>
@@ -3367,7 +3367,7 @@
       <c r="C38" s="27" t="n"/>
       <c r="D38" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E38" s="27" t="n"/>
@@ -3395,7 +3395,7 @@
       <c r="C39" s="27" t="n"/>
       <c r="D39" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E39" s="27" t="n"/>
@@ -3423,7 +3423,7 @@
       <c r="C40" s="27" t="n"/>
       <c r="D40" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E40" s="27" t="n"/>
@@ -3451,7 +3451,7 @@
       <c r="C41" s="27" t="n"/>
       <c r="D41" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E41" s="27" t="n"/>
@@ -3479,7 +3479,7 @@
       <c r="C42" s="27" t="n"/>
       <c r="D42" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E42" s="27" t="n"/>
@@ -3507,7 +3507,7 @@
       <c r="C43" s="27" t="n"/>
       <c r="D43" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E43" s="27" t="n"/>
@@ -3535,7 +3535,7 @@
       <c r="C44" s="27" t="n"/>
       <c r="D44" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E44" s="27" t="n"/>
@@ -3563,7 +3563,7 @@
       <c r="C45" s="27" t="n"/>
       <c r="D45" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E45" s="27" t="n"/>
@@ -3591,7 +3591,7 @@
       <c r="C46" s="27" t="n"/>
       <c r="D46" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E46" s="27" t="n"/>
@@ -3619,7 +3619,7 @@
       <c r="C47" s="27" t="n"/>
       <c r="D47" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E47" s="27" t="n"/>
@@ -5145,7 +5145,7 @@
       <c r="B35" s="28" t="n"/>
       <c r="C35" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D35" s="27" t="n"/>
@@ -5173,7 +5173,7 @@
       <c r="B36" s="28" t="n"/>
       <c r="C36" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D36" s="27" t="n"/>
@@ -5201,7 +5201,7 @@
       <c r="B37" s="28" t="n"/>
       <c r="C37" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D37" s="27" t="n"/>
@@ -5229,7 +5229,7 @@
       <c r="B38" s="27" t="n"/>
       <c r="C38" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D38" s="27" t="n"/>
@@ -5257,7 +5257,7 @@
       <c r="B39" s="27" t="n"/>
       <c r="C39" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D39" s="27" t="n"/>
@@ -5285,7 +5285,7 @@
       <c r="B40" s="27" t="n"/>
       <c r="C40" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D40" s="27" t="n"/>
@@ -5313,7 +5313,7 @@
       <c r="B41" s="27" t="n"/>
       <c r="C41" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D41" s="27" t="n"/>
@@ -5341,7 +5341,7 @@
       <c r="B42" s="27" t="n"/>
       <c r="C42" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D42" s="27" t="n"/>
@@ -5369,7 +5369,7 @@
       <c r="B43" s="27" t="n"/>
       <c r="C43" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D43" s="27" t="n"/>
@@ -5397,7 +5397,7 @@
       <c r="B44" s="27" t="n"/>
       <c r="C44" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D44" s="27" t="n"/>
@@ -6984,7 +6984,7 @@
       <c r="B35" s="28" t="n"/>
       <c r="C35" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D35" s="27" t="n"/>
@@ -7012,7 +7012,7 @@
       <c r="B36" s="28" t="n"/>
       <c r="C36" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D36" s="27" t="n"/>
@@ -7040,7 +7040,7 @@
       <c r="B37" s="28" t="n"/>
       <c r="C37" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D37" s="27" t="n"/>
@@ -7068,7 +7068,7 @@
       <c r="B38" s="27" t="n"/>
       <c r="C38" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D38" s="27" t="n"/>
@@ -7097,7 +7097,7 @@
       <c r="C39" s="27" t="n"/>
       <c r="D39" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle Machine</t>
         </is>
       </c>
       <c r="E39" s="27" t="n"/>
@@ -10615,7 +10615,7 @@
       </c>
       <c r="B35" s="28" t="inlineStr">
         <is>
-          <t>Amphi 4H</t>
+          <t>Amphi 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C35" s="27" t="n"/>
@@ -10643,12 +10643,12 @@
       </c>
       <c r="B36" s="28" t="inlineStr">
         <is>
-          <t>Amphi 4H</t>
+          <t>Amphi 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C36" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D36" s="27" t="n"/>
@@ -10675,12 +10675,12 @@
       </c>
       <c r="B37" s="28" t="inlineStr">
         <is>
-          <t>Amphi 4H</t>
+          <t>Amphi 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C37" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D37" s="27" t="n"/>
@@ -10707,17 +10707,17 @@
       </c>
       <c r="B38" s="27" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C38" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D38" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E38" s="27" t="n"/>
@@ -10743,17 +10743,17 @@
       </c>
       <c r="B39" s="27" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C39" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D39" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E39" s="27" t="n"/>
@@ -10779,17 +10779,17 @@
       </c>
       <c r="B40" s="27" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C40" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D40" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle Machine</t>
         </is>
       </c>
       <c r="E40" s="27" t="n"/>
@@ -10816,12 +10816,12 @@
       <c r="B41" s="27" t="n"/>
       <c r="C41" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D41" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle Machine</t>
         </is>
       </c>
       <c r="E41" s="27" t="n"/>
@@ -10847,17 +10847,17 @@
       </c>
       <c r="B42" s="27" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C42" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D42" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle Machine</t>
         </is>
       </c>
       <c r="E42" s="27" t="n"/>
@@ -10884,12 +10884,12 @@
       <c r="B43" s="27" t="n"/>
       <c r="C43" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D43" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle Machine</t>
         </is>
       </c>
       <c r="E43" s="27" t="n"/>
@@ -10915,17 +10915,17 @@
       </c>
       <c r="B44" s="27" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C44" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D44" s="27" t="inlineStr">
         <is>
-          <t>TP 6H</t>
+          <t>TP 3H - Salle Machine</t>
         </is>
       </c>
       <c r="E44" s="27" t="n"/>
@@ -10952,12 +10952,12 @@
       <c r="B45" s="27" t="n"/>
       <c r="C45" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D45" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle Machine</t>
         </is>
       </c>
       <c r="E45" s="27" t="n"/>
@@ -10983,17 +10983,17 @@
       </c>
       <c r="B46" s="27" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C46" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle Machine</t>
         </is>
       </c>
       <c r="D46" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle Machine</t>
         </is>
       </c>
       <c r="E46" s="27" t="n"/>
@@ -11021,7 +11021,7 @@
       <c r="C47" s="27" t="n"/>
       <c r="D47" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E47" s="27" t="n"/>
@@ -11049,7 +11049,7 @@
       <c r="C48" s="27" t="n"/>
       <c r="D48" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E48" s="27" t="n"/>
@@ -11077,7 +11077,7 @@
       <c r="C49" s="27" t="n"/>
       <c r="D49" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E49" s="27" t="n"/>
@@ -11312,7 +11312,7 @@
     <row r="56">
       <c r="A56" s="24" t="inlineStr">
         <is>
-          <t>Alain Casali</t>
+          <t>CHRISTIAN ERNST</t>
         </is>
       </c>
       <c r="B56" s="66" t="n"/>
@@ -11333,13 +11333,13 @@
         <v>9</v>
       </c>
       <c r="M56" s="24" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="N56" s="21" t="n">
-        <v>152</v>
+        <v>76</v>
       </c>
       <c r="O56" s="24" t="n">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="P56" s="22" t="n">
         <v>1</v>
@@ -11350,7 +11350,7 @@
     <row r="57">
       <c r="A57" s="68" t="inlineStr">
         <is>
-          <t>Christian Ernst</t>
+          <t>BASMA BOUKENZE</t>
         </is>
       </c>
       <c r="B57" s="66" t="n"/>
@@ -11367,9 +11367,7 @@
       <c r="K57" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="L57" s="21" t="n">
-        <v>9</v>
-      </c>
+      <c r="L57" s="21" t="n"/>
       <c r="M57" s="24" t="n">
         <v>30</v>
       </c>
@@ -11386,11 +11384,7 @@
       <c r="R57" s="23" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="21" t="inlineStr">
-        <is>
-          <t>Basma Boukenze</t>
-        </is>
-      </c>
+      <c r="A58" s="21" t="n"/>
       <c r="B58" s="66" t="n"/>
       <c r="C58" s="21" t="n"/>
       <c r="D58" s="21" t="n"/>
@@ -11406,17 +11400,11 @@
         <v>0</v>
       </c>
       <c r="L58" s="21" t="n"/>
-      <c r="M58" s="21" t="n">
-        <v>30</v>
-      </c>
-      <c r="N58" s="21" t="n">
-        <v>76</v>
-      </c>
-      <c r="O58" s="21" t="n">
-        <v>38</v>
-      </c>
+      <c r="M58" s="21" t="n"/>
+      <c r="N58" s="21" t="n"/>
+      <c r="O58" s="21" t="n"/>
       <c r="P58" s="22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q58" s="23" t="n">
         <v>0</v>
@@ -11646,7 +11634,11 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="24" t="n"/>
+      <c r="A65" s="24" t="inlineStr">
+        <is>
+          <t>ALAIN CASALI</t>
+        </is>
+      </c>
       <c r="B65" s="66" t="n"/>
       <c r="C65" s="21" t="n"/>
       <c r="D65" s="21" t="n"/>
@@ -11661,11 +11653,21 @@
       <c r="K65" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="L65" s="24" t="n"/>
-      <c r="M65" s="24" t="n"/>
-      <c r="N65" s="21" t="n"/>
-      <c r="O65" s="24" t="n"/>
-      <c r="P65" s="22" t="n"/>
+      <c r="L65" s="24" t="n">
+        <v>9</v>
+      </c>
+      <c r="M65" s="24" t="n">
+        <v>60</v>
+      </c>
+      <c r="N65" s="21" t="n">
+        <v>152</v>
+      </c>
+      <c r="O65" s="24" t="n">
+        <v>76</v>
+      </c>
+      <c r="P65" s="22" t="n">
+        <v>1</v>
+      </c>
       <c r="Q65" s="23" t="n"/>
       <c r="R65" s="23" t="n"/>
     </row>
@@ -12604,7 +12606,7 @@
       </c>
       <c r="B35" s="28" t="inlineStr">
         <is>
-          <t>Amphi 4H</t>
+          <t>Amphi 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C35" s="27" t="n"/>
@@ -12632,13 +12634,13 @@
       </c>
       <c r="B36" s="28" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C36" s="27" t="n"/>
       <c r="D36" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E36" s="27" t="n"/>
@@ -12666,7 +12668,7 @@
       <c r="C37" s="27" t="n"/>
       <c r="D37" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E37" s="27" t="n"/>
@@ -12694,7 +12696,7 @@
       <c r="C38" s="27" t="n"/>
       <c r="D38" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E38" s="27" t="n"/>
@@ -12722,7 +12724,7 @@
       <c r="C39" s="27" t="n"/>
       <c r="D39" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E39" s="27" t="n"/>
@@ -14407,7 +14409,7 @@
       </c>
       <c r="B35" s="28" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C35" s="27" t="n"/>
@@ -14435,7 +14437,7 @@
       </c>
       <c r="B36" s="28" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C36" s="27" t="n"/>
@@ -14464,7 +14466,7 @@
       <c r="B37" s="28" t="n"/>
       <c r="C37" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle Machine</t>
         </is>
       </c>
       <c r="D37" s="27" t="n"/>
@@ -14493,7 +14495,7 @@
       <c r="C38" s="27" t="n"/>
       <c r="D38" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E38" s="27" t="n"/>
@@ -14521,7 +14523,7 @@
       <c r="C39" s="27" t="n"/>
       <c r="D39" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E39" s="27" t="n"/>
@@ -16210,13 +16212,13 @@
       </c>
       <c r="B35" s="28" t="inlineStr">
         <is>
-          <t>Amphi 4H</t>
+          <t>Amphi 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C35" s="27" t="n"/>
       <c r="D35" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E35" s="27" t="n"/>
@@ -16242,13 +16244,13 @@
       </c>
       <c r="B36" s="28" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C36" s="27" t="n"/>
       <c r="D36" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E36" s="27" t="n"/>
@@ -16269,14 +16271,14 @@
     <row r="37">
       <c r="A37" s="27" t="inlineStr">
         <is>
-          <t>2023-09-18</t>
+          <t>2023-09-25</t>
         </is>
       </c>
       <c r="B37" s="28" t="n"/>
       <c r="C37" s="27" t="n"/>
       <c r="D37" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E37" s="27" t="n"/>
@@ -16297,14 +16299,14 @@
     <row r="38">
       <c r="A38" s="27" t="inlineStr">
         <is>
-          <t>2023-09-25</t>
+          <t>2023-09-18</t>
         </is>
       </c>
       <c r="B38" s="27" t="n"/>
       <c r="C38" s="27" t="n"/>
       <c r="D38" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle Machine</t>
         </is>
       </c>
       <c r="E38" s="27" t="n"/>
@@ -16331,7 +16333,7 @@
       <c r="B39" s="27" t="n"/>
       <c r="C39" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle Machine</t>
         </is>
       </c>
       <c r="D39" s="27" t="n"/>
@@ -18017,7 +18019,7 @@
       </c>
       <c r="B35" s="28" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C35" s="27" t="n"/>
@@ -18045,7 +18047,7 @@
       </c>
       <c r="B36" s="28" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C36" s="27" t="n"/>
@@ -18073,13 +18075,13 @@
       </c>
       <c r="B37" s="28" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C37" s="27" t="n"/>
       <c r="D37" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E37" s="27" t="n"/>
@@ -18105,13 +18107,13 @@
       </c>
       <c r="B38" s="27" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C38" s="27" t="n"/>
       <c r="D38" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E38" s="27" t="n"/>
@@ -18137,13 +18139,13 @@
       </c>
       <c r="B39" s="27" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C39" s="27" t="n"/>
       <c r="D39" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E39" s="27" t="n"/>
@@ -18171,7 +18173,7 @@
       <c r="C40" s="27" t="n"/>
       <c r="D40" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E40" s="27" t="n"/>
@@ -18198,7 +18200,7 @@
       <c r="B41" s="27" t="n"/>
       <c r="C41" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D41" s="27" t="n"/>
@@ -18226,7 +18228,7 @@
       <c r="B42" s="27" t="n"/>
       <c r="C42" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D42" s="27" t="n"/>
@@ -18254,7 +18256,7 @@
       <c r="B43" s="27" t="n"/>
       <c r="C43" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle Machine</t>
         </is>
       </c>
       <c r="D43" s="27" t="n"/>
@@ -19861,7 +19863,7 @@
       <c r="B35" s="28" t="n"/>
       <c r="C35" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D35" s="27" t="n"/>
@@ -19889,7 +19891,7 @@
       <c r="B36" s="28" t="n"/>
       <c r="C36" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D36" s="27" t="n"/>
@@ -19917,7 +19919,7 @@
       <c r="B37" s="28" t="n"/>
       <c r="C37" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D37" s="27" t="n"/>
@@ -19945,7 +19947,7 @@
       <c r="B38" s="27" t="n"/>
       <c r="C38" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D38" s="27" t="n"/>
@@ -19974,7 +19976,7 @@
       <c r="C39" s="27" t="n"/>
       <c r="D39" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E39" s="27" t="n"/>
@@ -20002,7 +20004,7 @@
       <c r="C40" s="27" t="n"/>
       <c r="D40" s="27" t="inlineStr">
         <is>
-          <t>TP 4H</t>
+          <t>TP 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E40" s="27" t="n"/>
@@ -21668,7 +21670,7 @@
       <c r="B35" s="28" t="n"/>
       <c r="C35" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D35" s="27" t="n"/>
@@ -21695,12 +21697,12 @@
       </c>
       <c r="B36" s="28" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C36" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D36" s="27" t="n"/>
@@ -21727,12 +21729,12 @@
       </c>
       <c r="B37" s="28" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C37" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D37" s="27" t="n"/>
@@ -21760,7 +21762,7 @@
       <c r="B38" s="27" t="n"/>
       <c r="C38" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D38" s="27" t="n"/>
@@ -21788,7 +21790,7 @@
       <c r="B39" s="27" t="n"/>
       <c r="C39" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D39" s="27" t="n"/>
@@ -21816,7 +21818,7 @@
       <c r="B40" s="27" t="n"/>
       <c r="C40" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D40" s="27" t="n"/>
@@ -21844,7 +21846,7 @@
       <c r="B41" s="27" t="n"/>
       <c r="C41" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D41" s="27" t="n"/>
@@ -21872,12 +21874,12 @@
       <c r="B42" s="27" t="n"/>
       <c r="C42" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D42" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E42" s="27" t="n"/>
@@ -21905,7 +21907,7 @@
       <c r="C43" s="27" t="n"/>
       <c r="D43" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E43" s="27" t="n"/>
@@ -23510,12 +23512,12 @@
       </c>
       <c r="B35" s="28" t="inlineStr">
         <is>
-          <t>Amphi 2H</t>
+          <t>Amphi 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="C35" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D35" s="27" t="n"/>
@@ -23543,7 +23545,7 @@
       <c r="B36" s="28" t="n"/>
       <c r="C36" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D36" s="27" t="n"/>
@@ -23571,7 +23573,7 @@
       <c r="B37" s="28" t="n"/>
       <c r="C37" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D37" s="27" t="n"/>
@@ -23599,7 +23601,7 @@
       <c r="B38" s="27" t="n"/>
       <c r="C38" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D38" s="27" t="n"/>
@@ -23627,7 +23629,7 @@
       <c r="B39" s="27" t="n"/>
       <c r="C39" s="27" t="inlineStr">
         <is>
-          <t>TD 4H</t>
+          <t>TD 2H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D39" s="27" t="n"/>
@@ -23655,7 +23657,7 @@
       <c r="B40" s="27" t="n"/>
       <c r="C40" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D40" s="27" t="n"/>
@@ -23683,12 +23685,12 @@
       <c r="B41" s="27" t="n"/>
       <c r="C41" s="27" t="inlineStr">
         <is>
-          <t>TD 2H</t>
+          <t>TD 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="D41" s="27" t="inlineStr">
         <is>
-          <t>TP 2H</t>
+          <t>TP 1H - Salle TD/Amphi</t>
         </is>
       </c>
       <c r="E41" s="27" t="n"/>

</xml_diff>

<commit_message>
réglage bug ajout test cours
</commit_message>
<xml_diff>
--- a/SAE_3_01/fichiers genere/S1.xlsx
+++ b/SAE_3_01/fichiers genere/S1.xlsx
@@ -10792,7 +10792,11 @@
           <t>TP 2H</t>
         </is>
       </c>
-      <c r="E40" s="27" t="n"/>
+      <c r="E40" s="27" t="inlineStr">
+        <is>
+          <t>Test 2H</t>
+        </is>
+      </c>
       <c r="F40" s="27" t="n"/>
       <c r="G40" s="27" t="n"/>
       <c r="H40" s="27" t="n"/>
@@ -11104,7 +11108,11 @@
       <c r="B50" s="27" t="n"/>
       <c r="C50" s="27" t="n"/>
       <c r="D50" s="27" t="n"/>
-      <c r="E50" s="27" t="n"/>
+      <c r="E50" s="27" t="inlineStr">
+        <is>
+          <t>Test 2H</t>
+        </is>
+      </c>
       <c r="F50" s="27" t="n"/>
       <c r="G50" s="27" t="n"/>
       <c r="H50" s="27" t="n"/>
@@ -14582,7 +14590,11 @@
       <c r="B40" s="27" t="n"/>
       <c r="C40" s="27" t="n"/>
       <c r="D40" s="27" t="n"/>
-      <c r="E40" s="27" t="n"/>
+      <c r="E40" s="27" t="inlineStr">
+        <is>
+          <t>Test 4H</t>
+        </is>
+      </c>
       <c r="F40" s="27" t="n"/>
       <c r="G40" s="27" t="n"/>
       <c r="H40" s="27" t="n"/>
@@ -18208,7 +18220,11 @@
           <t>TP 4H</t>
         </is>
       </c>
-      <c r="E40" s="27" t="n"/>
+      <c r="E40" s="27" t="inlineStr">
+        <is>
+          <t>Test 2H</t>
+        </is>
+      </c>
       <c r="F40" s="27" t="n"/>
       <c r="G40" s="27" t="n"/>
       <c r="H40" s="27" t="n"/>
@@ -18292,7 +18308,11 @@
         </is>
       </c>
       <c r="D43" s="27" t="n"/>
-      <c r="E43" s="27" t="n"/>
+      <c r="E43" s="27" t="inlineStr">
+        <is>
+          <t>Test 2H</t>
+        </is>
+      </c>
       <c r="F43" s="27" t="n"/>
       <c r="G43" s="27" t="n"/>
       <c r="H43" s="27" t="n"/>

</xml_diff>

<commit_message>
jsp pq ça marche pas
</commit_message>
<xml_diff>
--- a/SAE_3_01/fichiers genere/S1.xlsx
+++ b/SAE_3_01/fichiers genere/S1.xlsx
@@ -2537,7 +2537,7 @@
       </c>
       <c r="G2" s="27" t="inlineStr">
         <is>
-          <t>JosÃ©e VAQUIERI PORTOLANO</t>
+          <t>Josée VAQUIERI PORTOLANO</t>
         </is>
       </c>
       <c r="H2" s="27" t="n"/>
@@ -11864,7 +11864,7 @@
       </c>
       <c r="G2" s="27" t="inlineStr">
         <is>
-          <t>MickaÃ«l MARTIN NEVOT</t>
+          <t>Mickaël MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="27" t="n"/>
@@ -13705,7 +13705,7 @@
       </c>
       <c r="G2" s="27" t="inlineStr">
         <is>
-          <t>MickaÃ«l MARTIN NEVOT</t>
+          <t>Mickaël MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="27" t="n"/>
@@ -15512,7 +15512,7 @@
       </c>
       <c r="G2" s="27" t="inlineStr">
         <is>
-          <t>MickaÃ«l MARTIN NEVOT</t>
+          <t>Mickaël MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="27" t="n"/>
@@ -17319,7 +17319,7 @@
       </c>
       <c r="G2" s="27" t="inlineStr">
         <is>
-          <t>MickaÃ«l MARTIN NEVOT</t>
+          <t>Mickaël MARTIN NEVOT</t>
         </is>
       </c>
       <c r="H2" s="27" t="n"/>

</xml_diff>

<commit_message>
ajout erreurs base de données etc
</commit_message>
<xml_diff>
--- a/SAE_3_01/fichiers genere/S1.xlsx
+++ b/SAE_3_01/fichiers genere/S1.xlsx
@@ -10002,7 +10002,11 @@
       <c r="R10" s="27" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="27" t="n"/>
+      <c r="A11" s="27" t="inlineStr">
+        <is>
+          <t>Alain Casali</t>
+        </is>
+      </c>
       <c r="B11" s="27" t="n"/>
       <c r="C11" s="27" t="n"/>
       <c r="D11" s="27" t="n"/>
@@ -10022,7 +10026,11 @@
       <c r="R11" s="27" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="27" t="n"/>
+      <c r="A12" s="27" t="inlineStr">
+        <is>
+          <t>Christian Ernst</t>
+        </is>
+      </c>
       <c r="B12" s="27" t="n"/>
       <c r="C12" s="27" t="n"/>
       <c r="D12" s="27" t="n"/>
@@ -10044,7 +10052,7 @@
     <row r="13" ht="29" customHeight="1">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>Répartition</t>
+          <t>Basma Boukenze</t>
         </is>
       </c>
       <c r="B13" s="5" t="inlineStr">
@@ -10161,7 +10169,7 @@
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
         <is>
-          <t>TD</t>
+          <t>Alain Casali</t>
         </is>
       </c>
       <c r="B17" s="12" t="n"/>
@@ -10185,7 +10193,7 @@
     <row r="18">
       <c r="A18" s="8" t="inlineStr">
         <is>
-          <t>Alain Casali</t>
+          <t>Christian Ernst</t>
         </is>
       </c>
       <c r="B18" s="13" t="n">
@@ -10269,8 +10277,14 @@
       <c r="R20" s="27" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="n"/>
-      <c r="B21" s="10" t="n"/>
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>Alain Casali</t>
+        </is>
+      </c>
+      <c r="B21" s="10" t="n">
+        <v>2</v>
+      </c>
       <c r="C21" s="27" t="n"/>
       <c r="D21" s="40" t="inlineStr">
         <is>
@@ -10295,10 +10309,12 @@
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
         <is>
-          <t>TP dédoublés</t>
-        </is>
-      </c>
-      <c r="B22" s="12" t="n"/>
+          <t>Christian Ernst</t>
+        </is>
+      </c>
+      <c r="B22" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="C22" s="27" t="n"/>
       <c r="D22" s="32" t="inlineStr">
         <is>
@@ -10323,11 +10339,11 @@
     <row r="23">
       <c r="A23" s="8" t="inlineStr">
         <is>
-          <t>Alain Casali</t>
+          <t>Basma Boukenze</t>
         </is>
       </c>
       <c r="B23" s="8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C23" s="27" t="n"/>
       <c r="D23" s="27" t="n"/>
@@ -10397,8 +10413,14 @@
       <c r="R25" s="27" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="10" t="n"/>
-      <c r="B26" s="10" t="n"/>
+      <c r="A26" s="10" t="inlineStr">
+        <is>
+          <t>Alain Casali</t>
+        </is>
+      </c>
+      <c r="B26" s="10" t="n">
+        <v>4</v>
+      </c>
       <c r="C26" s="27" t="n"/>
       <c r="D26" s="27" t="n"/>
       <c r="E26" s="27" t="n"/>
@@ -10419,10 +10441,12 @@
     <row r="27">
       <c r="A27" s="6" t="inlineStr">
         <is>
-          <t>TP non dédoublés</t>
-        </is>
-      </c>
-      <c r="B27" s="12" t="n"/>
+          <t>Christian Ernst</t>
+        </is>
+      </c>
+      <c r="B27" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="C27" s="27" t="n"/>
       <c r="D27" s="37" t="inlineStr">
         <is>
@@ -10447,7 +10471,7 @@
     <row r="28">
       <c r="A28" s="8" t="inlineStr">
         <is>
-          <t>Alain Casali</t>
+          <t>Basma Boukenze</t>
         </is>
       </c>
       <c r="B28" s="13" t="n">
@@ -10520,8 +10544,14 @@
       <c r="R30" s="27" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="10" t="n"/>
-      <c r="B31" s="10" t="n"/>
+      <c r="A31" s="10" t="inlineStr">
+        <is>
+          <t>Alain Casali</t>
+        </is>
+      </c>
+      <c r="B31" s="10" t="n">
+        <v>2</v>
+      </c>
       <c r="C31" s="27" t="n"/>
       <c r="D31" s="64" t="n"/>
       <c r="E31" s="59" t="n"/>
@@ -10540,8 +10570,14 @@
       <c r="R31" s="27" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="27" t="n"/>
-      <c r="B32" s="27" t="n"/>
+      <c r="A32" s="27" t="inlineStr">
+        <is>
+          <t>Christian Ernst</t>
+        </is>
+      </c>
+      <c r="B32" s="27" t="n">
+        <v>1</v>
+      </c>
       <c r="C32" s="27" t="n"/>
       <c r="D32" s="27" t="n"/>
       <c r="E32" s="27" t="n"/>
@@ -10562,13 +10598,11 @@
     <row r="33">
       <c r="A33" s="36" t="inlineStr">
         <is>
-          <t>Organisation détaillée</t>
-        </is>
-      </c>
-      <c r="B33" s="28" t="inlineStr">
-        <is>
-          <t>(toutes les informations doivent figurer ici)</t>
-        </is>
+          <t>Basma Boukenze</t>
+        </is>
+      </c>
+      <c r="B33" s="28" t="n">
+        <v>1</v>
       </c>
       <c r="C33" s="27" t="n"/>
       <c r="D33" s="27" t="n"/>
@@ -11373,7 +11407,9 @@
       <c r="K57" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="L57" s="21" t="n"/>
+      <c r="L57" s="21" t="n">
+        <v>12</v>
+      </c>
       <c r="M57" s="24" t="n">
         <v>30</v>
       </c>
@@ -11388,7 +11424,11 @@
       <c r="R57" s="23" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="21" t="n"/>
+      <c r="A58" s="21" t="inlineStr">
+        <is>
+          <t>CHRISTIAN ERNST</t>
+        </is>
+      </c>
       <c r="B58" s="66" t="n"/>
       <c r="C58" s="21" t="n"/>
       <c r="D58" s="21" t="n"/>
@@ -11404,9 +11444,15 @@
         <v>0</v>
       </c>
       <c r="L58" s="21" t="n"/>
-      <c r="M58" s="21" t="n"/>
-      <c r="N58" s="21" t="n"/>
-      <c r="O58" s="21" t="n"/>
+      <c r="M58" s="21" t="n">
+        <v>30</v>
+      </c>
+      <c r="N58" s="21" t="n">
+        <v>76</v>
+      </c>
+      <c r="O58" s="21" t="n">
+        <v>38</v>
+      </c>
       <c r="P58" s="22" t="n">
         <v>0</v>
       </c>
@@ -11418,7 +11464,11 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="21" t="n"/>
+      <c r="A59" s="21" t="inlineStr">
+        <is>
+          <t>BASMA BOUKENZE</t>
+        </is>
+      </c>
       <c r="B59" s="66" t="n"/>
       <c r="C59" s="21" t="n"/>
       <c r="D59" s="21" t="n"/>
@@ -11434,9 +11484,15 @@
         <v>0</v>
       </c>
       <c r="L59" s="21" t="n"/>
-      <c r="M59" s="21" t="n"/>
-      <c r="N59" s="21" t="n"/>
-      <c r="O59" s="21" t="n"/>
+      <c r="M59" s="21" t="n">
+        <v>30</v>
+      </c>
+      <c r="N59" s="21" t="n">
+        <v>76</v>
+      </c>
+      <c r="O59" s="21" t="n">
+        <v>38</v>
+      </c>
       <c r="P59" s="22" t="n">
         <v>0</v>
       </c>
@@ -11674,7 +11730,11 @@
       <c r="R65" s="23" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="21" t="n"/>
+      <c r="A66" s="21" t="inlineStr">
+        <is>
+          <t>ALAIN CASALI</t>
+        </is>
+      </c>
       <c r="B66" s="66" t="n"/>
       <c r="C66" s="21" t="n"/>
       <c r="D66" s="21" t="n"/>
@@ -11689,10 +11749,18 @@
       <c r="K66" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="L66" s="21" t="n"/>
-      <c r="M66" s="21" t="n"/>
-      <c r="N66" s="21" t="n"/>
-      <c r="O66" s="21" t="n"/>
+      <c r="L66" s="21" t="n">
+        <v>12</v>
+      </c>
+      <c r="M66" s="21" t="n">
+        <v>60</v>
+      </c>
+      <c r="N66" s="21" t="n">
+        <v>152</v>
+      </c>
+      <c r="O66" s="21" t="n">
+        <v>76</v>
+      </c>
       <c r="P66" s="22" t="n">
         <v>0</v>
       </c>
@@ -13183,7 +13251,7 @@
     <row r="56">
       <c r="A56" s="24" t="inlineStr">
         <is>
-          <t>CHRISTIAN LAKHAL</t>
+          <t>TEST2</t>
         </is>
       </c>
       <c r="B56" s="66" t="n"/>
@@ -13217,7 +13285,11 @@
       <c r="R56" s="23" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="68" t="n"/>
+      <c r="A57" s="68" t="inlineStr">
+        <is>
+          <t>CHRISTIAN LAKHAL</t>
+        </is>
+      </c>
       <c r="B57" s="66" t="n"/>
       <c r="C57" s="21" t="n"/>
       <c r="D57" s="21" t="n"/>

</xml_diff>

<commit_message>
ajout de la base de données, de l'ajout des erreurs dans la BD...
</commit_message>
<xml_diff>
--- a/SAE_3_01/fichiers genere/S1.xlsx
+++ b/SAE_3_01/fichiers genere/S1.xlsx
@@ -10002,11 +10002,7 @@
       <c r="R10" s="27" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="27" t="inlineStr">
-        <is>
-          <t>Alain Casali</t>
-        </is>
-      </c>
+      <c r="A11" s="27" t="n"/>
       <c r="B11" s="27" t="n"/>
       <c r="C11" s="27" t="n"/>
       <c r="D11" s="27" t="n"/>
@@ -10026,11 +10022,7 @@
       <c r="R11" s="27" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="27" t="inlineStr">
-        <is>
-          <t>Christian Ernst</t>
-        </is>
-      </c>
+      <c r="A12" s="27" t="n"/>
       <c r="B12" s="27" t="n"/>
       <c r="C12" s="27" t="n"/>
       <c r="D12" s="27" t="n"/>
@@ -10052,7 +10044,7 @@
     <row r="13" ht="29" customHeight="1">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>Basma Boukenze</t>
+          <t>Répartition</t>
         </is>
       </c>
       <c r="B13" s="5" t="inlineStr">
@@ -10169,7 +10161,7 @@
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
         <is>
-          <t>Alain Casali</t>
+          <t>TD</t>
         </is>
       </c>
       <c r="B17" s="12" t="n"/>
@@ -10193,7 +10185,7 @@
     <row r="18">
       <c r="A18" s="8" t="inlineStr">
         <is>
-          <t>Christian Ernst</t>
+          <t>Alain Casali</t>
         </is>
       </c>
       <c r="B18" s="13" t="n">
@@ -10277,14 +10269,8 @@
       <c r="R20" s="27" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="inlineStr">
-        <is>
-          <t>Alain Casali</t>
-        </is>
-      </c>
-      <c r="B21" s="10" t="n">
-        <v>2</v>
-      </c>
+      <c r="A21" s="10" t="n"/>
+      <c r="B21" s="10" t="n"/>
       <c r="C21" s="27" t="n"/>
       <c r="D21" s="40" t="inlineStr">
         <is>
@@ -10309,12 +10295,10 @@
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
         <is>
-          <t>Christian Ernst</t>
-        </is>
-      </c>
-      <c r="B22" s="12" t="n">
-        <v>1</v>
-      </c>
+          <t>TP dédoublés</t>
+        </is>
+      </c>
+      <c r="B22" s="12" t="n"/>
       <c r="C22" s="27" t="n"/>
       <c r="D22" s="32" t="inlineStr">
         <is>
@@ -10339,11 +10323,11 @@
     <row r="23">
       <c r="A23" s="8" t="inlineStr">
         <is>
-          <t>Basma Boukenze</t>
+          <t>Alain Casali</t>
         </is>
       </c>
       <c r="B23" s="8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C23" s="27" t="n"/>
       <c r="D23" s="27" t="n"/>
@@ -10413,14 +10397,8 @@
       <c r="R25" s="27" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="10" t="inlineStr">
-        <is>
-          <t>Alain Casali</t>
-        </is>
-      </c>
-      <c r="B26" s="10" t="n">
-        <v>4</v>
-      </c>
+      <c r="A26" s="10" t="n"/>
+      <c r="B26" s="10" t="n"/>
       <c r="C26" s="27" t="n"/>
       <c r="D26" s="27" t="n"/>
       <c r="E26" s="27" t="n"/>
@@ -10441,12 +10419,10 @@
     <row r="27">
       <c r="A27" s="6" t="inlineStr">
         <is>
-          <t>Christian Ernst</t>
-        </is>
-      </c>
-      <c r="B27" s="12" t="n">
-        <v>2</v>
-      </c>
+          <t>TP non dédoublés</t>
+        </is>
+      </c>
+      <c r="B27" s="12" t="n"/>
       <c r="C27" s="27" t="n"/>
       <c r="D27" s="37" t="inlineStr">
         <is>
@@ -10471,7 +10447,7 @@
     <row r="28">
       <c r="A28" s="8" t="inlineStr">
         <is>
-          <t>Basma Boukenze</t>
+          <t>Alain Casali</t>
         </is>
       </c>
       <c r="B28" s="13" t="n">
@@ -10544,14 +10520,8 @@
       <c r="R30" s="27" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="10" t="inlineStr">
-        <is>
-          <t>Alain Casali</t>
-        </is>
-      </c>
-      <c r="B31" s="10" t="n">
-        <v>2</v>
-      </c>
+      <c r="A31" s="10" t="n"/>
+      <c r="B31" s="10" t="n"/>
       <c r="C31" s="27" t="n"/>
       <c r="D31" s="64" t="n"/>
       <c r="E31" s="59" t="n"/>
@@ -10570,14 +10540,8 @@
       <c r="R31" s="27" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="27" t="inlineStr">
-        <is>
-          <t>Christian Ernst</t>
-        </is>
-      </c>
-      <c r="B32" s="27" t="n">
-        <v>1</v>
-      </c>
+      <c r="A32" s="27" t="n"/>
+      <c r="B32" s="27" t="n"/>
       <c r="C32" s="27" t="n"/>
       <c r="D32" s="27" t="n"/>
       <c r="E32" s="27" t="n"/>
@@ -10598,11 +10562,13 @@
     <row r="33">
       <c r="A33" s="36" t="inlineStr">
         <is>
-          <t>Basma Boukenze</t>
-        </is>
-      </c>
-      <c r="B33" s="28" t="n">
-        <v>1</v>
+          <t>Organisation détaillée</t>
+        </is>
+      </c>
+      <c r="B33" s="28" t="inlineStr">
+        <is>
+          <t>(toutes les informations doivent figurer ici)</t>
+        </is>
       </c>
       <c r="C33" s="27" t="n"/>
       <c r="D33" s="27" t="n"/>
@@ -11407,9 +11373,7 @@
       <c r="K57" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="L57" s="21" t="n">
-        <v>12</v>
-      </c>
+      <c r="L57" s="21" t="n"/>
       <c r="M57" s="24" t="n">
         <v>30</v>
       </c>
@@ -11424,11 +11388,7 @@
       <c r="R57" s="23" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="21" t="inlineStr">
-        <is>
-          <t>CHRISTIAN ERNST</t>
-        </is>
-      </c>
+      <c r="A58" s="21" t="n"/>
       <c r="B58" s="66" t="n"/>
       <c r="C58" s="21" t="n"/>
       <c r="D58" s="21" t="n"/>
@@ -11444,15 +11404,9 @@
         <v>0</v>
       </c>
       <c r="L58" s="21" t="n"/>
-      <c r="M58" s="21" t="n">
-        <v>30</v>
-      </c>
-      <c r="N58" s="21" t="n">
-        <v>76</v>
-      </c>
-      <c r="O58" s="21" t="n">
-        <v>38</v>
-      </c>
+      <c r="M58" s="21" t="n"/>
+      <c r="N58" s="21" t="n"/>
+      <c r="O58" s="21" t="n"/>
       <c r="P58" s="22" t="n">
         <v>0</v>
       </c>
@@ -11464,11 +11418,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="21" t="inlineStr">
-        <is>
-          <t>BASMA BOUKENZE</t>
-        </is>
-      </c>
+      <c r="A59" s="21" t="n"/>
       <c r="B59" s="66" t="n"/>
       <c r="C59" s="21" t="n"/>
       <c r="D59" s="21" t="n"/>
@@ -11484,15 +11434,9 @@
         <v>0</v>
       </c>
       <c r="L59" s="21" t="n"/>
-      <c r="M59" s="21" t="n">
-        <v>30</v>
-      </c>
-      <c r="N59" s="21" t="n">
-        <v>76</v>
-      </c>
-      <c r="O59" s="21" t="n">
-        <v>38</v>
-      </c>
+      <c r="M59" s="21" t="n"/>
+      <c r="N59" s="21" t="n"/>
+      <c r="O59" s="21" t="n"/>
       <c r="P59" s="22" t="n">
         <v>0</v>
       </c>
@@ -11730,11 +11674,7 @@
       <c r="R65" s="23" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="21" t="inlineStr">
-        <is>
-          <t>ALAIN CASALI</t>
-        </is>
-      </c>
+      <c r="A66" s="21" t="n"/>
       <c r="B66" s="66" t="n"/>
       <c r="C66" s="21" t="n"/>
       <c r="D66" s="21" t="n"/>
@@ -11749,18 +11689,10 @@
       <c r="K66" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="L66" s="21" t="n">
-        <v>12</v>
-      </c>
-      <c r="M66" s="21" t="n">
-        <v>60</v>
-      </c>
-      <c r="N66" s="21" t="n">
-        <v>152</v>
-      </c>
-      <c r="O66" s="21" t="n">
-        <v>76</v>
-      </c>
+      <c r="L66" s="21" t="n"/>
+      <c r="M66" s="21" t="n"/>
+      <c r="N66" s="21" t="n"/>
+      <c r="O66" s="21" t="n"/>
       <c r="P66" s="22" t="n">
         <v>0</v>
       </c>
@@ -13251,7 +13183,7 @@
     <row r="56">
       <c r="A56" s="24" t="inlineStr">
         <is>
-          <t>TEST2</t>
+          <t>CHRISTIAN LAKHAL</t>
         </is>
       </c>
       <c r="B56" s="66" t="n"/>
@@ -13285,11 +13217,7 @@
       <c r="R56" s="23" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="68" t="inlineStr">
-        <is>
-          <t>CHRISTIAN LAKHAL</t>
-        </is>
-      </c>
+      <c r="A57" s="68" t="n"/>
       <c r="B57" s="66" t="n"/>
       <c r="C57" s="21" t="n"/>
       <c r="D57" s="21" t="n"/>

</xml_diff>